<commit_message>
Gestion cond paiement et facturation
</commit_message>
<xml_diff>
--- a/data/Suivi CA licences et maintenance 2023.xlsx
+++ b/data/Suivi CA licences et maintenance 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrunoQUEGUINER\OneDrive - SEENOVATE\Bureau\PCOE\app-pcoe\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seenovatecom-my.sharepoint.com/personal/remy_fouchereau_seenovate_com/Documents/Documents/GitHub/app-pcoe/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4DDD07-B3E1-4F3B-AC1D-70A3D42EEEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{EF4DDD07-B3E1-4F3B-AC1D-70A3D42EEEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{992B4253-9978-48B8-B3D6-077667C549F0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-16260" windowWidth="29040" windowHeight="15720" tabRatio="627" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="627" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Client ex OEM" sheetId="10" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Abonnement Cloud'!$B$4:$AC$56</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Maintenance SAP BusinessObjects'!$A$1:$AX$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Maintenance SAP BusinessObjects'!$A$1:$AZ$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Résiliations PCOE'!$A$3:$M$3</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -152,7 +152,7 @@
     <author>tc={EEF44DC3-7189-4A10-B227-F51E10CBFA76}</author>
   </authors>
   <commentList>
-    <comment ref="U5" authorId="0" shapeId="0" xr:uid="{5EE1CFCA-3B8F-40CC-86CC-CD25FD4705E2}">
+    <comment ref="W5" authorId="0" shapeId="0" xr:uid="{5EE1CFCA-3B8F-40CC-86CC-CD25FD4705E2}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="290">
   <si>
     <t>SUIVI DES COMPTES OEM</t>
   </si>
@@ -1055,6 +1055,15 @@
   </si>
   <si>
     <t>BAI SA (BRITTANY FERRIES) - Replication Server</t>
+  </si>
+  <si>
+    <t>Condition de paiement</t>
+  </si>
+  <si>
+    <t>Condition de facturation</t>
+  </si>
+  <si>
+    <t>gratuit</t>
   </si>
 </sst>
 </file>
@@ -2885,7 +2894,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U5" dT="2022-12-20T10:29:29.67" personId="{C5D2CC8A-44EF-403A-9BFA-0EDEDBDF960E}" id="{5EE1CFCA-3B8F-40CC-86CC-CD25FD4705E2}">
+  <threadedComment ref="W5" dT="2022-12-20T10:29:29.67" personId="{C5D2CC8A-44EF-403A-9BFA-0EDEDBDF960E}" id="{5EE1CFCA-3B8F-40CC-86CC-CD25FD4705E2}">
     <text>Le client a payé directement sans facture !!!</text>
   </threadedComment>
   <threadedComment ref="G13" dT="2022-11-04T16:10:32.58" personId="{E7A34A8E-C034-469E-849C-6BCB5949BFF3}" id="{349EA861-622B-4834-BACB-A6FD3C12C6CD}">
@@ -2914,15 +2923,15 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:31" s="6" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:31" s="6" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3"/>
       <c r="B3" s="102"/>
       <c r="C3" s="294" t="s">
@@ -2957,7 +2966,7 @@
       <c r="AD3" s="102"/>
       <c r="AE3" s="102"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B10" s="292" t="s">
         <v>1</v>
       </c>
@@ -2974,7 +2983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
         <v>6</v>
       </c>
@@ -2991,28 +3000,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="293" t="s">
         <v>10</v>
       </c>
@@ -3029,21 +3038,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="293"/>
       <c r="C18" s="293"/>
       <c r="D18" s="293"/>
       <c r="E18" s="293"/>
       <c r="F18" s="293"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="293"/>
       <c r="C19" s="293"/>
       <c r="D19" s="293"/>
       <c r="E19" s="293"/>
       <c r="F19" s="293"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
         <v>13</v>
       </c>
@@ -3052,21 +3061,21 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="293" t="s">
         <v>14</v>
       </c>
@@ -3075,21 +3084,21 @@
       <c r="E23" s="293"/>
       <c r="F23" s="293"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="293"/>
       <c r="C24" s="293"/>
       <c r="D24" s="293"/>
       <c r="E24" s="293"/>
       <c r="F24" s="293"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="293"/>
       <c r="C25" s="293"/>
       <c r="D25" s="293"/>
       <c r="E25" s="293"/>
       <c r="F25" s="293"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
         <v>15</v>
       </c>
@@ -3098,21 +3107,21 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="293" t="s">
         <v>16</v>
       </c>
@@ -3121,21 +3130,21 @@
       <c r="E29" s="293"/>
       <c r="F29" s="293"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="293"/>
       <c r="C30" s="293"/>
       <c r="D30" s="293"/>
       <c r="E30" s="293"/>
       <c r="F30" s="293"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="293"/>
       <c r="C31" s="293"/>
       <c r="D31" s="293"/>
       <c r="E31" s="293"/>
       <c r="F31" s="293"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="293"/>
       <c r="C32" s="293"/>
       <c r="D32" s="293"/>
@@ -3163,37 +3172,37 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="102"/>
-    <col min="2" max="2" width="42.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="10" customWidth="1"/>
-    <col min="4" max="6" width="14.42578125" style="102" customWidth="1"/>
-    <col min="7" max="9" width="13.42578125" style="102" customWidth="1"/>
-    <col min="10" max="12" width="12.42578125" style="102" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="102" customWidth="1"/>
-    <col min="14" max="14" width="51.42578125" style="12" customWidth="1"/>
-    <col min="15" max="15" width="32.42578125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" style="12" customWidth="1"/>
-    <col min="17" max="19" width="2.42578125" style="102" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" style="102" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="102"/>
+    <col min="2" max="2" width="42.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="10" customWidth="1"/>
+    <col min="4" max="6" width="14.44140625" style="102" customWidth="1"/>
+    <col min="7" max="9" width="13.44140625" style="102" customWidth="1"/>
+    <col min="10" max="12" width="12.44140625" style="102" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="102" customWidth="1"/>
+    <col min="14" max="14" width="51.44140625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="32.44140625" style="12" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" style="12" customWidth="1"/>
+    <col min="17" max="19" width="2.44140625" style="102" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" style="102" customWidth="1"/>
     <col min="21" max="21" width="13" style="102" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" style="103" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" style="102" customWidth="1"/>
+    <col min="22" max="22" width="13.44140625" style="103" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" style="102" customWidth="1"/>
     <col min="24" max="24" width="15" style="102" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="18" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="12.44140625" style="18" customWidth="1"/>
     <col min="27" max="27" width="13" style="102" customWidth="1"/>
     <col min="28" max="28" width="13" style="103" customWidth="1"/>
-    <col min="29" max="29" width="47.42578125" style="102" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" style="104"/>
-    <col min="31" max="31" width="12.42578125" style="104" customWidth="1"/>
-    <col min="32" max="41" width="10.42578125" style="102"/>
-    <col min="42" max="43" width="11.42578125" style="102" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="10.42578125" style="102"/>
+    <col min="29" max="29" width="47.44140625" style="102" customWidth="1"/>
+    <col min="30" max="30" width="10.44140625" style="104"/>
+    <col min="31" max="31" width="12.44140625" style="104" customWidth="1"/>
+    <col min="32" max="41" width="10.44140625" style="102"/>
+    <col min="42" max="43" width="11.44140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="10.44140625" style="102"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:53" ht="90.75" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:53" ht="90" x14ac:dyDescent="0.5">
       <c r="E2" s="21" t="s">
         <v>17</v>
       </c>
@@ -3212,7 +3221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D3" s="305" t="s">
         <v>19</v>
       </c>
@@ -3273,7 +3282,7 @@
       <c r="AZ3" s="304"/>
       <c r="BA3" s="304"/>
     </row>
-    <row r="4" spans="1:53" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>25</v>
       </c>
@@ -3434,7 +3443,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="15" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" s="15" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="94"/>
       <c r="B5" s="15" t="s">
         <v>65</v>
@@ -3551,7 +3560,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="6" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="151" t="s">
         <v>66</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="151" t="s">
         <v>66</v>
       </c>
@@ -3837,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="151" t="s">
         <v>72</v>
       </c>
@@ -3991,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="151" t="s">
         <v>72</v>
       </c>
@@ -4145,7 +4154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="151" t="s">
         <v>66</v>
       </c>
@@ -4297,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="151" t="s">
         <v>72</v>
       </c>
@@ -4458,7 +4467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="151" t="s">
         <v>66</v>
       </c>
@@ -4608,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="151" t="s">
         <v>72</v>
       </c>
@@ -4769,7 +4778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="151" t="s">
         <v>72</v>
       </c>
@@ -4927,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="151" t="s">
         <v>72</v>
       </c>
@@ -5085,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="151" t="s">
         <v>72</v>
       </c>
@@ -5239,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="151" t="s">
         <v>72</v>
       </c>
@@ -5393,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="151" t="s">
         <v>72</v>
       </c>
@@ -5545,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="151" t="s">
         <v>72</v>
       </c>
@@ -5696,7 +5705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="223" t="s">
         <v>72</v>
       </c>
@@ -5852,7 +5861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="223" t="s">
         <v>66</v>
       </c>
@@ -5996,7 +6005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="71" t="s">
         <v>72</v>
       </c>
@@ -6153,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
         <v>72</v>
       </c>
@@ -6309,7 +6318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="71" t="s">
         <v>72</v>
       </c>
@@ -6466,7 +6475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="87" t="s">
         <v>66</v>
       </c>
@@ -6593,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="71" t="s">
         <v>72</v>
       </c>
@@ -6724,7 +6733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="71" t="s">
         <v>66</v>
       </c>
@@ -6860,7 +6869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="71" t="s">
         <v>66</v>
       </c>
@@ -7018,7 +7027,7 @@
         <v>201750</v>
       </c>
     </row>
-    <row r="29" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="71" t="s">
         <v>66</v>
       </c>
@@ -7155,7 +7164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="71" t="s">
         <v>66</v>
       </c>
@@ -7292,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="71" t="s">
         <v>111</v>
       </c>
@@ -7442,7 +7451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="71" t="s">
         <v>115</v>
       </c>
@@ -7597,7 +7606,7 @@
         <v>33501.660000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="71" t="s">
         <v>66</v>
       </c>
@@ -7756,7 +7765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="71" t="s">
         <v>66</v>
       </c>
@@ -7915,7 +7924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="71" t="s">
         <v>126</v>
       </c>
@@ -8065,7 +8074,7 @@
         <v>43912</v>
       </c>
     </row>
-    <row r="36" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="71" t="s">
         <v>111</v>
       </c>
@@ -8217,7 +8226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="71" t="s">
         <v>72</v>
       </c>
@@ -8350,7 +8359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="71" t="s">
         <v>66</v>
       </c>
@@ -8489,7 +8498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="71" t="s">
         <v>66</v>
       </c>
@@ -8644,7 +8653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="71" t="s">
         <v>66</v>
       </c>
@@ -8791,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="71" t="s">
         <v>72</v>
       </c>
@@ -8957,7 +8966,7 @@
         <v>33600</v>
       </c>
     </row>
-    <row r="42" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="71" t="s">
         <v>72</v>
       </c>
@@ -9118,7 +9127,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="43" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="71" t="s">
         <v>66</v>
       </c>
@@ -9249,7 +9258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="71" t="s">
         <v>66</v>
       </c>
@@ -9397,7 +9406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="71" t="s">
         <v>66</v>
       </c>
@@ -9534,7 +9543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="71" t="s">
         <v>115</v>
       </c>
@@ -9679,7 +9688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="71" t="s">
         <v>115</v>
       </c>
@@ -9824,7 +9833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="71" t="s">
         <v>111</v>
       </c>
@@ -9974,7 +9983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="71" t="s">
         <v>72</v>
       </c>
@@ -10121,7 +10130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="71"/>
       <c r="B50" s="86"/>
       <c r="C50" s="86"/>
@@ -10254,7 +10263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="71"/>
       <c r="B51" s="86"/>
       <c r="C51" s="86"/>
@@ -10387,7 +10396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="71"/>
       <c r="B52" s="86"/>
       <c r="C52" s="86"/>
@@ -10520,7 +10529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="71"/>
       <c r="B53" s="86" t="s">
         <v>155</v>
@@ -10655,7 +10664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="71"/>
       <c r="B54" s="88"/>
       <c r="C54" s="88"/>
@@ -10782,7 +10791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="99" t="s">
         <v>156</v>
       </c>
@@ -10924,7 +10933,7 @@
         <v>318163.66000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B56" s="99" t="s">
         <v>157</v>
       </c>
@@ -10948,147 +10957,147 @@
       <c r="H56" s="56"/>
       <c r="I56" s="56"/>
     </row>
-    <row r="57" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:53" x14ac:dyDescent="0.3">
       <c r="H57" s="56"/>
       <c r="I57" s="56"/>
     </row>
-    <row r="58" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="H58" s="56"/>
       <c r="I58" s="56"/>
     </row>
-    <row r="59" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:53" x14ac:dyDescent="0.3">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="H59" s="56"/>
       <c r="I59" s="56"/>
     </row>
-    <row r="60" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:53" x14ac:dyDescent="0.3">
       <c r="H60" s="56"/>
       <c r="I60" s="56"/>
     </row>
-    <row r="61" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:53" x14ac:dyDescent="0.3">
       <c r="H61" s="56"/>
       <c r="I61" s="56"/>
     </row>
-    <row r="62" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:53" x14ac:dyDescent="0.3">
       <c r="H62" s="56"/>
       <c r="I62" s="56"/>
     </row>
-    <row r="63" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:53" x14ac:dyDescent="0.3">
       <c r="H63" s="56"/>
       <c r="I63" s="56"/>
     </row>
-    <row r="64" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:53" x14ac:dyDescent="0.3">
       <c r="H64" s="56"/>
       <c r="I64" s="56"/>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H65"/>
       <c r="I65"/>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H66"/>
       <c r="I66"/>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H67"/>
       <c r="I67"/>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H68"/>
       <c r="I68"/>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H69"/>
       <c r="I69"/>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H70"/>
       <c r="I70"/>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H71"/>
       <c r="I71"/>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H72"/>
       <c r="I72"/>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H73"/>
       <c r="I73"/>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H74"/>
       <c r="I74"/>
     </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H75"/>
       <c r="I75"/>
     </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H76"/>
       <c r="I76"/>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H77"/>
       <c r="I77"/>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H78"/>
       <c r="I78"/>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H79"/>
       <c r="I79"/>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H80"/>
       <c r="I80"/>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H81"/>
       <c r="I81"/>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H82"/>
       <c r="I82"/>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H83"/>
       <c r="I83"/>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H84"/>
       <c r="I84"/>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H85"/>
       <c r="I85"/>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H86"/>
       <c r="I86"/>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H87"/>
       <c r="I87"/>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H88"/>
       <c r="I88"/>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H89"/>
       <c r="I89"/>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H90"/>
       <c r="I90"/>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H91"/>
       <c r="I91"/>
     </row>
@@ -11121,17 +11130,17 @@
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="18"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="18"/>
-    <col min="8" max="8" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="11.44140625" style="18"/>
+    <col min="2" max="2" width="50.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="18"/>
+    <col min="8" max="8" width="11.44140625" style="7"/>
     <col min="12" max="12" width="57" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:880" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:880" s="2" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="310"/>
       <c r="C1" s="310"/>
@@ -12015,7 +12024,7 @@
       <c r="AGU1" s="102"/>
       <c r="AGV1" s="102"/>
     </row>
-    <row r="2" spans="1:880" s="162" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:880" s="162" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="313"/>
       <c r="B2" s="313"/>
       <c r="C2" s="313"/>
@@ -12901,7 +12910,7 @@
       <c r="AGU2" s="217"/>
       <c r="AGV2" s="218"/>
     </row>
-    <row r="3" spans="1:880" s="168" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:880" s="168" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="163" t="s">
         <v>25</v>
       </c>
@@ -13809,7 +13818,7 @@
       <c r="AGU3" s="207"/>
       <c r="AGV3" s="205"/>
     </row>
-    <row r="4" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
         <v>111</v>
       </c>
@@ -13835,7 +13844,7 @@
       <c r="L4" s="199"/>
       <c r="M4" s="150"/>
     </row>
-    <row r="5" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="82" t="s">
         <v>66</v>
       </c>
@@ -13874,7 +13883,7 @@
       <c r="L5" s="200"/>
       <c r="M5" s="150"/>
     </row>
-    <row r="6" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="82" t="s">
         <v>66</v>
       </c>
@@ -13899,7 +13908,7 @@
       <c r="L6" s="200"/>
       <c r="M6" s="150"/>
     </row>
-    <row r="7" spans="1:880" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:880" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="82" t="s">
         <v>111</v>
       </c>
@@ -14796,7 +14805,7 @@
       <c r="AGT7"/>
       <c r="AGU7"/>
     </row>
-    <row r="8" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="82" t="s">
         <v>72</v>
       </c>
@@ -14831,7 +14840,7 @@
       </c>
       <c r="M8" s="150"/>
     </row>
-    <row r="9" spans="1:880" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:880" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="82" t="s">
         <v>72</v>
       </c>
@@ -15719,7 +15728,7 @@
       <c r="AGT9"/>
       <c r="AGU9"/>
     </row>
-    <row r="10" spans="1:880" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:880" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="82" t="s">
         <v>111</v>
       </c>
@@ -16609,7 +16618,7 @@
       <c r="AGT10"/>
       <c r="AGU10"/>
     </row>
-    <row r="11" spans="1:880" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:880" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="82" t="s">
         <v>72</v>
       </c>
@@ -17497,7 +17506,7 @@
       <c r="AGT11"/>
       <c r="AGU11"/>
     </row>
-    <row r="12" spans="1:880" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:880" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="82" t="s">
         <v>72</v>
       </c>
@@ -18385,7 +18394,7 @@
       <c r="AGT12"/>
       <c r="AGU12"/>
     </row>
-    <row r="13" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="82" t="s">
         <v>72</v>
       </c>
@@ -18412,7 +18421,7 @@
       <c r="L13" s="201"/>
       <c r="M13" s="150"/>
     </row>
-    <row r="14" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="204"/>
       <c r="B14" s="88" t="s">
         <v>182</v>
@@ -18434,7 +18443,7 @@
       <c r="L14" s="199"/>
       <c r="M14" s="150"/>
     </row>
-    <row r="15" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="82" t="s">
         <v>72</v>
       </c>
@@ -18459,7 +18468,7 @@
       <c r="L15" s="200"/>
       <c r="M15" s="150"/>
     </row>
-    <row r="16" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="82" t="s">
         <v>72</v>
       </c>
@@ -18484,7 +18493,7 @@
       <c r="L16" s="200"/>
       <c r="M16" s="150"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="82" t="s">
         <v>66</v>
       </c>
@@ -18517,7 +18526,7 @@
       <c r="L17" s="203"/>
       <c r="M17" s="150"/>
     </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="82" t="s">
         <v>66</v>
       </c>
@@ -18541,7 +18550,7 @@
       </c>
       <c r="M18" s="150"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="82" t="s">
         <v>72</v>
       </c>
@@ -18572,7 +18581,7 @@
       <c r="L19" s="200"/>
       <c r="M19" s="150"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="82" t="s">
         <v>66</v>
       </c>
@@ -18598,7 +18607,7 @@
       </c>
       <c r="M20" s="150"/>
     </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="82" t="s">
         <v>111</v>
       </c>
@@ -18622,7 +18631,7 @@
       <c r="L21" s="199"/>
       <c r="M21" s="150"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="204" t="s">
         <v>66</v>
       </c>
@@ -18648,7 +18657,7 @@
       <c r="L22" s="199"/>
       <c r="M22" s="150"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="204" t="s">
         <v>72</v>
       </c>
@@ -18670,7 +18679,7 @@
       <c r="L23" s="200"/>
       <c r="M23" s="150"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="82" t="s">
         <v>72</v>
       </c>
@@ -18694,7 +18703,7 @@
       <c r="L24" s="200"/>
       <c r="M24" s="150"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="204" t="s">
         <v>72</v>
       </c>
@@ -18717,7 +18726,7 @@
       </c>
       <c r="M25" s="150"/>
     </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="82" t="s">
         <v>66</v>
       </c>
@@ -18740,7 +18749,7 @@
       <c r="L26" s="199"/>
       <c r="M26" s="150"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="82" t="s">
         <v>111</v>
       </c>
@@ -18769,7 +18778,7 @@
       <c r="L27" s="199"/>
       <c r="M27" s="150"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="82" t="s">
         <v>72</v>
       </c>
@@ -18792,7 +18801,7 @@
       <c r="L28" s="200"/>
       <c r="M28" s="150"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="82" t="s">
         <v>66</v>
       </c>
@@ -18819,7 +18828,7 @@
       <c r="L29" s="203"/>
       <c r="M29" s="150"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="82" t="s">
         <v>72</v>
       </c>
@@ -18846,7 +18855,7 @@
       <c r="L30" s="200"/>
       <c r="M30" s="150"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="82" t="s">
         <v>111</v>
       </c>
@@ -18867,7 +18876,7 @@
       <c r="L31" s="199"/>
       <c r="M31" s="150"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="204" t="s">
         <v>66</v>
       </c>
@@ -18888,7 +18897,7 @@
       <c r="L32" s="199"/>
       <c r="M32" s="150"/>
     </row>
-    <row r="33" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="204" t="s">
         <v>66</v>
       </c>
@@ -18912,7 +18921,7 @@
       <c r="L33" s="199"/>
       <c r="M33" s="150"/>
     </row>
-    <row r="34" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="82" t="s">
         <v>66</v>
       </c>
@@ -18937,7 +18946,7 @@
       <c r="L34" s="199"/>
       <c r="M34" s="150"/>
     </row>
-    <row r="35" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="82" t="s">
         <v>72</v>
       </c>
@@ -18970,7 +18979,7 @@
       <c r="L35" s="200"/>
       <c r="M35" s="150"/>
     </row>
-    <row r="36" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="82" t="s">
         <v>72</v>
       </c>
@@ -19003,7 +19012,7 @@
       <c r="L36" s="200"/>
       <c r="M36" s="150"/>
     </row>
-    <row r="37" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="82" t="s">
         <v>72</v>
       </c>
@@ -19024,7 +19033,7 @@
       <c r="L37" s="200"/>
       <c r="M37" s="150"/>
     </row>
-    <row r="38" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="82" t="s">
         <v>72</v>
       </c>
@@ -19055,7 +19064,7 @@
       <c r="L38" s="200"/>
       <c r="M38" s="150"/>
     </row>
-    <row r="39" spans="1:880" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:880" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="82" t="s">
         <v>72</v>
       </c>
@@ -19080,7 +19089,7 @@
       <c r="L39" s="200"/>
       <c r="M39" s="150"/>
     </row>
-    <row r="40" spans="1:880" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:880" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="82" t="s">
         <v>72</v>
       </c>
@@ -19102,7 +19111,7 @@
       <c r="L40" s="202"/>
       <c r="M40" s="150"/>
     </row>
-    <row r="41" spans="1:880" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:880" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="82" t="s">
         <v>66</v>
       </c>
@@ -19995,7 +20004,7 @@
       <c r="AGU41"/>
       <c r="AGV41" s="206"/>
     </row>
-    <row r="42" spans="1:880" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:880" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="71" t="s">
         <v>111</v>
       </c>
@@ -20152,7 +20161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:880" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:880" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="71" t="s">
         <v>72</v>
       </c>
@@ -20307,7 +20316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:880" s="87" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:880" s="87" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="82" t="s">
         <v>72</v>
       </c>
@@ -20482,54 +20491,54 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AZ61"/>
+  <dimension ref="A1:BB61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" style="10" customWidth="1"/>
-    <col min="3" max="4" width="13.42578125" style="144" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" customWidth="1"/>
-    <col min="6" max="8" width="14.42578125" style="2" customWidth="1"/>
-    <col min="9" max="11" width="13.42578125" style="2" customWidth="1"/>
-    <col min="12" max="13" width="12.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="181" customWidth="1"/>
-    <col min="15" max="15" width="24.42578125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13" style="2" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="3" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="17.42578125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="7" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" style="18" customWidth="1"/>
-    <col min="24" max="24" width="13" style="2" customWidth="1"/>
-    <col min="25" max="25" width="13" style="3" customWidth="1"/>
-    <col min="26" max="26" width="47.42578125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5703125" style="4" customWidth="1"/>
-    <col min="29" max="29" width="13.85546875" style="2" customWidth="1"/>
-    <col min="30" max="30" width="12" style="2" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" style="2" customWidth="1"/>
-    <col min="32" max="32" width="17.7109375" style="2" customWidth="1"/>
-    <col min="33" max="33" width="12.7109375" style="2" customWidth="1"/>
-    <col min="34" max="34" width="18.85546875" style="2" customWidth="1"/>
-    <col min="35" max="35" width="19.85546875" style="2" customWidth="1"/>
-    <col min="36" max="36" width="10.42578125" style="2"/>
-    <col min="37" max="37" width="18.140625" style="2" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" style="2"/>
-    <col min="39" max="40" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="10.42578125" style="2"/>
+    <col min="1" max="1" width="14.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.44140625" style="10" customWidth="1"/>
+    <col min="3" max="4" width="13.44140625" style="144" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="2" customWidth="1"/>
+    <col min="6" max="8" width="14.44140625" style="2" customWidth="1"/>
+    <col min="9" max="11" width="13.44140625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="12.44140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" style="181" customWidth="1"/>
+    <col min="15" max="15" width="24.44140625" style="12" customWidth="1"/>
+    <col min="16" max="18" width="11.44140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.44140625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="13" style="2" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="14.44140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="17.44140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="17.109375" style="7" customWidth="1"/>
+    <col min="25" max="25" width="12.44140625" style="18" customWidth="1"/>
+    <col min="26" max="26" width="13" style="2" customWidth="1"/>
+    <col min="27" max="27" width="13" style="3" customWidth="1"/>
+    <col min="28" max="28" width="47.44140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" style="4" customWidth="1"/>
+    <col min="31" max="31" width="13.88671875" style="2" customWidth="1"/>
+    <col min="32" max="32" width="12" style="2" customWidth="1"/>
+    <col min="33" max="33" width="10.6640625" style="2" customWidth="1"/>
+    <col min="34" max="34" width="17.6640625" style="2" customWidth="1"/>
+    <col min="35" max="35" width="12.6640625" style="2" customWidth="1"/>
+    <col min="36" max="36" width="18.88671875" style="2" customWidth="1"/>
+    <col min="37" max="37" width="19.88671875" style="2" customWidth="1"/>
+    <col min="38" max="38" width="10.44140625" style="2"/>
+    <col min="39" max="39" width="18.109375" style="2" customWidth="1"/>
+    <col min="40" max="40" width="10.44140625" style="2"/>
+    <col min="41" max="42" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="10.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="168" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" s="168" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="163" t="s">
         <v>25</v>
       </c>
@@ -20578,72 +20587,76 @@
       <c r="P1" s="166" t="s">
         <v>166</v>
       </c>
-      <c r="Q1" s="167" t="s">
+      <c r="Q1" s="166" t="s">
+        <v>287</v>
+      </c>
+      <c r="R1" s="166" t="s">
+        <v>288</v>
+      </c>
+      <c r="S1" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="167" t="s">
+      <c r="T1" s="167" t="s">
         <v>230</v>
       </c>
-      <c r="S1" s="167" t="s">
+      <c r="U1" s="167" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="167" t="s">
+      <c r="V1" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="167" t="s">
+      <c r="W1" s="167" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="167" t="s">
+      <c r="X1" s="167" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="167" t="s">
+      <c r="Y1" s="167" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="167" t="s">
+      <c r="Z1" s="167" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="167" t="s">
+      <c r="AA1" s="167" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="153" t="s">
+      <c r="AB1" s="153" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="154" t="s">
+      <c r="AC1" s="154" t="s">
         <v>231</v>
       </c>
-      <c r="AB1" s="154" t="s">
+      <c r="AD1" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="AC1" s="154" t="s">
+      <c r="AE1" s="154" t="s">
         <v>233</v>
       </c>
-      <c r="AD1" s="154" t="s">
+      <c r="AF1" s="154" t="s">
         <v>234</v>
       </c>
-      <c r="AE1" s="154" t="s">
+      <c r="AG1" s="154" t="s">
         <v>235</v>
       </c>
-      <c r="AF1" s="154" t="s">
+      <c r="AH1" s="154" t="s">
         <v>236</v>
       </c>
-      <c r="AG1" s="154" t="s">
+      <c r="AI1" s="154" t="s">
         <v>237</v>
       </c>
-      <c r="AH1" s="154" t="s">
+      <c r="AJ1" s="154" t="s">
         <v>238</v>
       </c>
-      <c r="AI1" s="154" t="s">
+      <c r="AK1" s="154" t="s">
         <v>239</v>
       </c>
-      <c r="AJ1" s="154" t="s">
+      <c r="AL1" s="154" t="s">
         <v>240</v>
       </c>
-      <c r="AK1" s="154" t="s">
+      <c r="AM1" s="154" t="s">
         <v>241</v>
       </c>
-      <c r="AL1" s="154"/>
-      <c r="AM1" s="155"/>
-      <c r="AN1" s="155"/>
+      <c r="AN1" s="154"/>
       <c r="AO1" s="155"/>
       <c r="AP1" s="155"/>
       <c r="AQ1" s="155"/>
@@ -20654,8 +20667,10 @@
       <c r="AV1" s="155"/>
       <c r="AW1" s="155"/>
       <c r="AX1" s="155"/>
+      <c r="AY1" s="155"/>
+      <c r="AZ1" s="155"/>
     </row>
-    <row r="2" spans="1:50" s="177" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" s="177" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
         <v>72</v>
       </c>
@@ -20708,38 +20723,42 @@
       <c r="P2" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q2" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R2" s="302">
-        <v>44197</v>
+      <c r="Q2" s="150" t="s">
+        <v>289</v>
+      </c>
+      <c r="R2" s="150" t="s">
+        <v>289</v>
       </c>
       <c r="S2" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T2" s="212">
+      <c r="T2" s="302">
+        <v>44197</v>
+      </c>
+      <c r="U2" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V2" s="212">
         <v>44900</v>
       </c>
-      <c r="U2" s="212">
+      <c r="W2" s="212">
         <v>44565</v>
       </c>
-      <c r="V2" s="69" t="s">
+      <c r="X2" s="69" t="s">
         <v>246</v>
       </c>
-      <c r="W2" s="303">
+      <c r="Y2" s="303">
         <v>44197</v>
       </c>
-      <c r="X2" s="120" t="s">
+      <c r="Z2" s="120" t="s">
         <v>247</v>
       </c>
-      <c r="Y2" s="120" t="s">
+      <c r="AA2" s="120" t="s">
         <v>248</v>
       </c>
-      <c r="Z2" s="70" t="s">
+      <c r="AB2" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
@@ -20750,8 +20769,8 @@
       <c r="AJ2" s="27"/>
       <c r="AK2" s="27"/>
       <c r="AL2" s="27"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
       <c r="AO2" s="37"/>
       <c r="AP2" s="37"/>
       <c r="AQ2" s="37"/>
@@ -20762,8 +20781,10 @@
       <c r="AV2" s="37"/>
       <c r="AW2" s="37"/>
       <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
     </row>
-    <row r="3" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="71" t="s">
         <v>66</v>
       </c>
@@ -20810,24 +20831,24 @@
       <c r="P3" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="120" t="s">
+      <c r="Q3" s="150"/>
+      <c r="R3" s="150"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T3" s="213">
+      <c r="V3" s="213">
         <v>44902</v>
       </c>
-      <c r="U3" s="213">
+      <c r="W3" s="213">
         <v>44902</v>
       </c>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
       <c r="X3" s="69"/>
       <c r="Y3" s="69"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="69"/>
+      <c r="AB3" s="70"/>
       <c r="AC3" s="27"/>
       <c r="AD3" s="27"/>
       <c r="AE3" s="27"/>
@@ -20838,8 +20859,8 @@
       <c r="AJ3" s="27"/>
       <c r="AK3" s="27"/>
       <c r="AL3" s="27"/>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="37"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="27"/>
       <c r="AO3" s="37"/>
       <c r="AP3" s="37"/>
       <c r="AQ3" s="37"/>
@@ -20850,8 +20871,10 @@
       <c r="AV3" s="37"/>
       <c r="AW3" s="37"/>
       <c r="AX3" s="37"/>
+      <c r="AY3" s="37"/>
+      <c r="AZ3" s="37"/>
     </row>
-    <row r="4" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
         <v>72</v>
       </c>
@@ -20898,24 +20921,24 @@
       <c r="P4" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="120" t="s">
+      <c r="Q4" s="150"/>
+      <c r="R4" s="150"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T4" s="212">
+      <c r="V4" s="212">
         <v>44900</v>
       </c>
-      <c r="U4" s="212">
+      <c r="W4" s="212">
         <v>44900</v>
       </c>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
       <c r="X4" s="81"/>
       <c r="Y4" s="81"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="78"/>
       <c r="AC4" s="27"/>
       <c r="AD4" s="27"/>
       <c r="AE4" s="27"/>
@@ -20926,8 +20949,8 @@
       <c r="AJ4" s="27"/>
       <c r="AK4" s="27"/>
       <c r="AL4" s="27"/>
-      <c r="AM4" s="37"/>
-      <c r="AN4" s="37"/>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="27"/>
       <c r="AO4" s="37"/>
       <c r="AP4" s="37"/>
       <c r="AQ4" s="37"/>
@@ -20938,8 +20961,10 @@
       <c r="AV4" s="37"/>
       <c r="AW4" s="37"/>
       <c r="AX4" s="37"/>
+      <c r="AY4" s="37"/>
+      <c r="AZ4" s="37"/>
     </row>
-    <row r="5" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="71" t="s">
         <v>111</v>
       </c>
@@ -20986,26 +21011,26 @@
       <c r="P5" s="150" t="s">
         <v>220</v>
       </c>
-      <c r="Q5" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R5" s="120"/>
+      <c r="Q5" s="150"/>
+      <c r="R5" s="150"/>
       <c r="S5" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T5" s="215">
+      <c r="T5" s="120"/>
+      <c r="U5" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V5" s="215">
         <v>44895</v>
       </c>
-      <c r="U5" s="215">
+      <c r="W5" s="215">
         <v>44915</v>
       </c>
-      <c r="V5" s="121"/>
-      <c r="W5" s="121"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="122"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
+      <c r="X5" s="121"/>
+      <c r="Y5" s="121"/>
+      <c r="Z5" s="64"/>
+      <c r="AA5" s="122"/>
+      <c r="AB5" s="70"/>
       <c r="AC5" s="27"/>
       <c r="AD5" s="27"/>
       <c r="AE5" s="27"/>
@@ -21016,8 +21041,8 @@
       <c r="AJ5" s="27"/>
       <c r="AK5" s="27"/>
       <c r="AL5" s="27"/>
-      <c r="AM5" s="37"/>
-      <c r="AN5" s="37"/>
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="27"/>
       <c r="AO5" s="37"/>
       <c r="AP5" s="37"/>
       <c r="AQ5" s="37"/>
@@ -21028,8 +21053,10 @@
       <c r="AV5" s="37"/>
       <c r="AW5" s="37"/>
       <c r="AX5" s="37"/>
+      <c r="AY5" s="37"/>
+      <c r="AZ5" s="37"/>
     </row>
-    <row r="6" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="71" t="s">
         <v>72</v>
       </c>
@@ -21076,24 +21103,24 @@
       <c r="P6" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q6" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R6" s="81"/>
+      <c r="Q6" s="150"/>
+      <c r="R6" s="150"/>
       <c r="S6" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T6" s="212">
+      <c r="T6" s="81"/>
+      <c r="U6" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V6" s="212">
         <v>44900</v>
       </c>
-      <c r="U6" s="214"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
+      <c r="W6" s="214"/>
       <c r="X6" s="81"/>
       <c r="Y6" s="81"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="27"/>
+      <c r="Z6" s="81"/>
+      <c r="AA6" s="81"/>
+      <c r="AB6" s="78"/>
       <c r="AC6" s="27"/>
       <c r="AD6" s="27"/>
       <c r="AE6" s="27"/>
@@ -21104,8 +21131,8 @@
       <c r="AJ6" s="27"/>
       <c r="AK6" s="27"/>
       <c r="AL6" s="27"/>
-      <c r="AM6" s="37"/>
-      <c r="AN6" s="37"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="27"/>
       <c r="AO6" s="37"/>
       <c r="AP6" s="37"/>
       <c r="AQ6" s="37"/>
@@ -21116,8 +21143,10 @@
       <c r="AV6" s="37"/>
       <c r="AW6" s="37"/>
       <c r="AX6" s="37"/>
+      <c r="AY6" s="37"/>
+      <c r="AZ6" s="37"/>
     </row>
-    <row r="7" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="71" t="s">
         <v>72</v>
       </c>
@@ -21164,26 +21193,26 @@
       <c r="P7" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q7" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R7" s="81"/>
+      <c r="Q7" s="150"/>
+      <c r="R7" s="150"/>
       <c r="S7" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T7" s="212">
+      <c r="T7" s="81"/>
+      <c r="U7" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V7" s="212">
         <v>44900</v>
       </c>
-      <c r="U7" s="214">
+      <c r="W7" s="214">
         <v>44902</v>
       </c>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
       <c r="X7" s="81"/>
       <c r="Y7" s="81"/>
-      <c r="Z7" s="78"/>
-      <c r="AA7" s="27"/>
-      <c r="AB7" s="27"/>
+      <c r="Z7" s="81"/>
+      <c r="AA7" s="81"/>
+      <c r="AB7" s="78"/>
       <c r="AC7" s="27"/>
       <c r="AD7" s="27"/>
       <c r="AE7" s="27"/>
@@ -21194,8 +21223,8 @@
       <c r="AJ7" s="27"/>
       <c r="AK7" s="27"/>
       <c r="AL7" s="27"/>
-      <c r="AM7" s="37"/>
-      <c r="AN7" s="37"/>
+      <c r="AM7" s="27"/>
+      <c r="AN7" s="27"/>
       <c r="AO7" s="37"/>
       <c r="AP7" s="37"/>
       <c r="AQ7" s="37"/>
@@ -21206,8 +21235,10 @@
       <c r="AV7" s="37"/>
       <c r="AW7" s="37"/>
       <c r="AX7" s="37"/>
+      <c r="AY7" s="37"/>
+      <c r="AZ7" s="37"/>
     </row>
-    <row r="8" spans="1:50" s="171" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" s="171" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="71" t="s">
         <v>72</v>
       </c>
@@ -21256,24 +21287,24 @@
       <c r="P8" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="120" t="s">
+      <c r="Q8" s="150"/>
+      <c r="R8" s="150"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T8" s="214">
+      <c r="V8" s="214">
         <v>44900</v>
       </c>
-      <c r="U8" s="214">
+      <c r="W8" s="214">
         <v>44902</v>
       </c>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
       <c r="X8" s="81"/>
       <c r="Y8" s="81"/>
-      <c r="Z8" s="78"/>
-      <c r="AA8" s="27"/>
-      <c r="AB8" s="27"/>
+      <c r="Z8" s="81"/>
+      <c r="AA8" s="81"/>
+      <c r="AB8" s="78"/>
       <c r="AC8" s="27"/>
       <c r="AD8" s="27"/>
       <c r="AE8" s="27"/>
@@ -21284,8 +21315,8 @@
       <c r="AJ8" s="27"/>
       <c r="AK8" s="27"/>
       <c r="AL8" s="27"/>
-      <c r="AM8" s="37"/>
-      <c r="AN8" s="37"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
       <c r="AO8" s="37"/>
       <c r="AP8" s="37"/>
       <c r="AQ8" s="37"/>
@@ -21296,8 +21327,10 @@
       <c r="AV8" s="37"/>
       <c r="AW8" s="37"/>
       <c r="AX8" s="37"/>
+      <c r="AY8" s="37"/>
+      <c r="AZ8" s="37"/>
     </row>
-    <row r="9" spans="1:50" s="171" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" s="171" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="71" t="s">
         <v>72</v>
       </c>
@@ -21344,26 +21377,26 @@
       <c r="P9" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q9" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R9" s="69"/>
+      <c r="Q9" s="150"/>
+      <c r="R9" s="150"/>
       <c r="S9" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T9" s="212">
+      <c r="T9" s="69"/>
+      <c r="U9" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V9" s="212">
         <v>44900</v>
       </c>
-      <c r="U9" s="213">
+      <c r="W9" s="213">
         <v>44956</v>
       </c>
-      <c r="V9" s="69"/>
-      <c r="W9" s="69"/>
       <c r="X9" s="69"/>
       <c r="Y9" s="69"/>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="70"/>
       <c r="AC9" s="27"/>
       <c r="AD9" s="27"/>
       <c r="AE9" s="27"/>
@@ -21374,8 +21407,8 @@
       <c r="AJ9" s="27"/>
       <c r="AK9" s="27"/>
       <c r="AL9" s="27"/>
-      <c r="AM9" s="37"/>
-      <c r="AN9" s="37"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="27"/>
       <c r="AO9" s="37"/>
       <c r="AP9" s="37"/>
       <c r="AQ9" s="37"/>
@@ -21386,8 +21419,10 @@
       <c r="AV9" s="37"/>
       <c r="AW9" s="37"/>
       <c r="AX9" s="37"/>
+      <c r="AY9" s="37"/>
+      <c r="AZ9" s="37"/>
     </row>
-    <row r="10" spans="1:50" s="170" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" s="170" customFormat="1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="71" t="s">
         <v>72</v>
       </c>
@@ -21434,24 +21469,24 @@
       <c r="P10" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="120" t="s">
+      <c r="Q10" s="150"/>
+      <c r="R10" s="150"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T10" s="213">
+      <c r="V10" s="213">
         <v>44907</v>
       </c>
-      <c r="U10" s="213">
+      <c r="W10" s="213">
         <v>44910</v>
       </c>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
       <c r="X10" s="69"/>
       <c r="Y10" s="69"/>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
+      <c r="Z10" s="69"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="70"/>
       <c r="AC10" s="27"/>
       <c r="AD10" s="27"/>
       <c r="AE10" s="27"/>
@@ -21462,8 +21497,8 @@
       <c r="AJ10" s="27"/>
       <c r="AK10" s="27"/>
       <c r="AL10" s="27"/>
-      <c r="AM10" s="37"/>
-      <c r="AN10" s="37"/>
+      <c r="AM10" s="27"/>
+      <c r="AN10" s="27"/>
       <c r="AO10" s="37"/>
       <c r="AP10" s="37"/>
       <c r="AQ10" s="37"/>
@@ -21474,8 +21509,10 @@
       <c r="AV10" s="37"/>
       <c r="AW10" s="37"/>
       <c r="AX10" s="37"/>
+      <c r="AY10" s="37"/>
+      <c r="AZ10" s="37"/>
     </row>
-    <row r="11" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="71" t="s">
         <v>72</v>
       </c>
@@ -21522,24 +21559,24 @@
       <c r="P11" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q11" s="69"/>
-      <c r="R11" s="69"/>
-      <c r="S11" s="120" t="s">
+      <c r="Q11" s="150"/>
+      <c r="R11" s="150"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T11" s="213">
+      <c r="V11" s="213">
         <v>44907</v>
       </c>
-      <c r="U11" s="213">
+      <c r="W11" s="213">
         <v>44910</v>
       </c>
-      <c r="V11" s="69"/>
-      <c r="W11" s="69"/>
       <c r="X11" s="69"/>
       <c r="Y11" s="69"/>
-      <c r="Z11" s="70"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
+      <c r="Z11" s="69"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="70"/>
       <c r="AC11" s="27"/>
       <c r="AD11" s="27"/>
       <c r="AE11" s="27"/>
@@ -21550,8 +21587,8 @@
       <c r="AJ11" s="27"/>
       <c r="AK11" s="27"/>
       <c r="AL11" s="27"/>
-      <c r="AM11" s="37"/>
-      <c r="AN11" s="37"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="27"/>
       <c r="AO11" s="37"/>
       <c r="AP11" s="37"/>
       <c r="AQ11" s="37"/>
@@ -21562,8 +21599,10 @@
       <c r="AV11" s="37"/>
       <c r="AW11" s="37"/>
       <c r="AX11" s="37"/>
+      <c r="AY11" s="37"/>
+      <c r="AZ11" s="37"/>
     </row>
-    <row r="12" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="71" t="s">
         <v>66</v>
       </c>
@@ -21609,24 +21648,24 @@
       <c r="P12" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="Q12" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R12" s="81"/>
+      <c r="Q12" s="150"/>
+      <c r="R12" s="150"/>
       <c r="S12" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T12" s="214"/>
-      <c r="U12" s="214">
+      <c r="T12" s="81"/>
+      <c r="U12" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V12" s="214"/>
+      <c r="W12" s="214">
         <v>44938</v>
       </c>
-      <c r="V12" s="81"/>
-      <c r="W12" s="81"/>
       <c r="X12" s="81"/>
       <c r="Y12" s="81"/>
-      <c r="Z12" s="78"/>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="27"/>
+      <c r="Z12" s="81"/>
+      <c r="AA12" s="81"/>
+      <c r="AB12" s="78"/>
       <c r="AC12" s="27"/>
       <c r="AD12" s="27"/>
       <c r="AE12" s="27"/>
@@ -21637,8 +21676,8 @@
       <c r="AJ12" s="27"/>
       <c r="AK12" s="27"/>
       <c r="AL12" s="27"/>
-      <c r="AM12" s="37"/>
-      <c r="AN12" s="37"/>
+      <c r="AM12" s="27"/>
+      <c r="AN12" s="27"/>
       <c r="AO12" s="37"/>
       <c r="AP12" s="37"/>
       <c r="AQ12" s="37"/>
@@ -21649,8 +21688,10 @@
       <c r="AV12" s="37"/>
       <c r="AW12" s="37"/>
       <c r="AX12" s="37"/>
+      <c r="AY12" s="37"/>
+      <c r="AZ12" s="37"/>
     </row>
-    <row r="13" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="58" t="s">
         <v>72</v>
       </c>
@@ -21697,22 +21738,22 @@
       <c r="P13" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q13" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R13" s="81"/>
+      <c r="Q13" s="150"/>
+      <c r="R13" s="150"/>
       <c r="S13" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T13" s="214"/>
-      <c r="U13" s="214"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="81"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V13" s="214"/>
+      <c r="W13" s="214"/>
       <c r="X13" s="81"/>
       <c r="Y13" s="81"/>
-      <c r="Z13" s="78"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
+      <c r="Z13" s="81"/>
+      <c r="AA13" s="81"/>
+      <c r="AB13" s="78"/>
       <c r="AC13" s="27"/>
       <c r="AD13" s="27"/>
       <c r="AE13" s="27"/>
@@ -21723,8 +21764,8 @@
       <c r="AJ13" s="27"/>
       <c r="AK13" s="27"/>
       <c r="AL13" s="27"/>
-      <c r="AM13" s="37"/>
-      <c r="AN13" s="37"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="27"/>
       <c r="AO13" s="37"/>
       <c r="AP13" s="37"/>
       <c r="AQ13" s="37"/>
@@ -21735,8 +21776,10 @@
       <c r="AV13" s="37"/>
       <c r="AW13" s="37"/>
       <c r="AX13" s="37"/>
+      <c r="AY13" s="37"/>
+      <c r="AZ13" s="37"/>
     </row>
-    <row r="14" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="58" t="s">
         <v>72</v>
       </c>
@@ -21781,22 +21824,22 @@
       <c r="P14" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q14" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R14" s="81"/>
+      <c r="Q14" s="150"/>
+      <c r="R14" s="150"/>
       <c r="S14" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T14" s="214"/>
-      <c r="U14" s="214"/>
-      <c r="V14" s="81"/>
-      <c r="W14" s="81"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V14" s="214"/>
+      <c r="W14" s="214"/>
       <c r="X14" s="81"/>
       <c r="Y14" s="81"/>
-      <c r="Z14" s="78"/>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="27"/>
+      <c r="Z14" s="81"/>
+      <c r="AA14" s="81"/>
+      <c r="AB14" s="78"/>
       <c r="AC14" s="27"/>
       <c r="AD14" s="27"/>
       <c r="AE14" s="27"/>
@@ -21807,8 +21850,8 @@
       <c r="AJ14" s="27"/>
       <c r="AK14" s="27"/>
       <c r="AL14" s="27"/>
-      <c r="AM14" s="37"/>
-      <c r="AN14" s="37"/>
+      <c r="AM14" s="27"/>
+      <c r="AN14" s="27"/>
       <c r="AO14" s="37"/>
       <c r="AP14" s="37"/>
       <c r="AQ14" s="37"/>
@@ -21819,8 +21862,10 @@
       <c r="AV14" s="37"/>
       <c r="AW14" s="37"/>
       <c r="AX14" s="37"/>
+      <c r="AY14" s="37"/>
+      <c r="AZ14" s="37"/>
     </row>
-    <row r="15" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="71" t="s">
         <v>111</v>
       </c>
@@ -21867,24 +21912,24 @@
       <c r="P15" s="150" t="s">
         <v>220</v>
       </c>
-      <c r="Q15" s="120"/>
-      <c r="R15" s="64" t="s">
+      <c r="Q15" s="150"/>
+      <c r="R15" s="150"/>
+      <c r="S15" s="120"/>
+      <c r="T15" s="64" t="s">
         <v>264</v>
       </c>
-      <c r="S15" s="120" t="s">
+      <c r="U15" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T15" s="215">
+      <c r="V15" s="215">
         <v>44895</v>
       </c>
-      <c r="U15" s="215"/>
-      <c r="V15" s="121"/>
-      <c r="W15" s="125"/>
-      <c r="X15" s="58"/>
-      <c r="Y15" s="122"/>
-      <c r="Z15" s="70"/>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
+      <c r="W15" s="215"/>
+      <c r="X15" s="121"/>
+      <c r="Y15" s="125"/>
+      <c r="Z15" s="58"/>
+      <c r="AA15" s="122"/>
+      <c r="AB15" s="70"/>
       <c r="AC15" s="27"/>
       <c r="AD15" s="27"/>
       <c r="AE15" s="27"/>
@@ -21895,8 +21940,8 @@
       <c r="AJ15" s="27"/>
       <c r="AK15" s="27"/>
       <c r="AL15" s="27"/>
-      <c r="AM15" s="37"/>
-      <c r="AN15" s="37"/>
+      <c r="AM15" s="27"/>
+      <c r="AN15" s="27"/>
       <c r="AO15" s="37"/>
       <c r="AP15" s="37"/>
       <c r="AQ15" s="37"/>
@@ -21907,8 +21952,10 @@
       <c r="AV15" s="37"/>
       <c r="AW15" s="37"/>
       <c r="AX15" s="37"/>
+      <c r="AY15" s="37"/>
+      <c r="AZ15" s="37"/>
     </row>
-    <row r="16" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="71" t="s">
         <v>66</v>
       </c>
@@ -21955,28 +22002,28 @@
       <c r="P16" s="150" t="s">
         <v>266</v>
       </c>
-      <c r="Q16" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R16" s="120"/>
+      <c r="Q16" s="150"/>
+      <c r="R16" s="150"/>
       <c r="S16" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T16" s="214">
+      <c r="T16" s="120"/>
+      <c r="U16" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V16" s="214">
         <v>44910</v>
       </c>
-      <c r="U16" s="212">
+      <c r="W16" s="212">
         <v>44932</v>
       </c>
-      <c r="V16" s="69" t="s">
+      <c r="X16" s="69" t="s">
         <v>267</v>
       </c>
-      <c r="W16" s="69"/>
-      <c r="X16" s="69"/>
       <c r="Y16" s="69"/>
-      <c r="Z16" s="70"/>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="27"/>
+      <c r="Z16" s="69"/>
+      <c r="AA16" s="69"/>
+      <c r="AB16" s="70"/>
       <c r="AC16" s="27"/>
       <c r="AD16" s="27"/>
       <c r="AE16" s="27"/>
@@ -21987,8 +22034,8 @@
       <c r="AJ16" s="27"/>
       <c r="AK16" s="27"/>
       <c r="AL16" s="27"/>
-      <c r="AM16" s="37"/>
-      <c r="AN16" s="37"/>
+      <c r="AM16" s="27"/>
+      <c r="AN16" s="27"/>
       <c r="AO16" s="37"/>
       <c r="AP16" s="37"/>
       <c r="AQ16" s="37"/>
@@ -21999,8 +22046,10 @@
       <c r="AV16" s="37"/>
       <c r="AW16" s="37"/>
       <c r="AX16" s="37"/>
+      <c r="AY16" s="37"/>
+      <c r="AZ16" s="37"/>
     </row>
-    <row r="17" spans="1:50" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" s="82" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="82" t="s">
         <v>66</v>
       </c>
@@ -22049,28 +22098,28 @@
       <c r="P17" s="287" t="s">
         <v>266</v>
       </c>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="81"/>
-      <c r="S17" s="81" t="s">
+      <c r="Q17" s="287"/>
+      <c r="R17" s="287"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81" t="s">
         <v>221</v>
       </c>
-      <c r="T17" s="214">
+      <c r="V17" s="214">
         <v>44910</v>
       </c>
-      <c r="U17" s="213">
+      <c r="W17" s="213">
         <v>44932</v>
       </c>
-      <c r="V17" s="81" t="s">
+      <c r="X17" s="81" t="s">
         <v>267</v>
       </c>
-      <c r="W17" s="81"/>
-      <c r="X17" s="81"/>
       <c r="Y17" s="81"/>
-      <c r="Z17" s="83" t="s">
+      <c r="Z17" s="81"/>
+      <c r="AA17" s="81"/>
+      <c r="AB17" s="83" t="s">
         <v>269</v>
       </c>
-      <c r="AA17" s="288"/>
-      <c r="AB17" s="288"/>
       <c r="AC17" s="288"/>
       <c r="AD17" s="288"/>
       <c r="AE17" s="288"/>
@@ -22081,8 +22130,8 @@
       <c r="AJ17" s="288"/>
       <c r="AK17" s="288"/>
       <c r="AL17" s="288"/>
-      <c r="AM17" s="289"/>
-      <c r="AN17" s="289"/>
+      <c r="AM17" s="288"/>
+      <c r="AN17" s="288"/>
       <c r="AO17" s="289"/>
       <c r="AP17" s="289"/>
       <c r="AQ17" s="289"/>
@@ -22093,8 +22142,10 @@
       <c r="AV17" s="289"/>
       <c r="AW17" s="289"/>
       <c r="AX17" s="289"/>
+      <c r="AY17" s="289"/>
+      <c r="AZ17" s="289"/>
     </row>
-    <row r="18" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="71" t="s">
         <v>66</v>
       </c>
@@ -22140,26 +22191,26 @@
       <c r="P18" s="150" t="s">
         <v>266</v>
       </c>
-      <c r="Q18" s="120"/>
-      <c r="R18" s="120"/>
-      <c r="S18" s="120" t="s">
+      <c r="Q18" s="150"/>
+      <c r="R18" s="150"/>
+      <c r="S18" s="120"/>
+      <c r="T18" s="120"/>
+      <c r="U18" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T18" s="214">
+      <c r="V18" s="214">
         <v>44910</v>
       </c>
-      <c r="U18" s="212">
+      <c r="W18" s="212">
         <v>44929</v>
       </c>
-      <c r="V18" s="69" t="s">
+      <c r="X18" s="69" t="s">
         <v>271</v>
       </c>
-      <c r="W18" s="69"/>
-      <c r="X18" s="69"/>
       <c r="Y18" s="69"/>
-      <c r="Z18" s="70"/>
-      <c r="AA18" s="27"/>
-      <c r="AB18" s="27"/>
+      <c r="Z18" s="69"/>
+      <c r="AA18" s="69"/>
+      <c r="AB18" s="70"/>
       <c r="AC18" s="27"/>
       <c r="AD18" s="27"/>
       <c r="AE18" s="27"/>
@@ -22170,8 +22221,8 @@
       <c r="AJ18" s="27"/>
       <c r="AK18" s="27"/>
       <c r="AL18" s="27"/>
-      <c r="AM18" s="37"/>
-      <c r="AN18" s="37"/>
+      <c r="AM18" s="27"/>
+      <c r="AN18" s="27"/>
       <c r="AO18" s="37"/>
       <c r="AP18" s="37"/>
       <c r="AQ18" s="37"/>
@@ -22182,8 +22233,10 @@
       <c r="AV18" s="37"/>
       <c r="AW18" s="37"/>
       <c r="AX18" s="37"/>
+      <c r="AY18" s="37"/>
+      <c r="AZ18" s="37"/>
     </row>
-    <row r="19" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="173" t="s">
         <v>111</v>
       </c>
@@ -22229,26 +22282,26 @@
       <c r="P19" s="150" t="s">
         <v>220</v>
       </c>
-      <c r="Q19" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R19" s="120"/>
+      <c r="Q19" s="150"/>
+      <c r="R19" s="150"/>
       <c r="S19" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T19" s="215">
+      <c r="T19" s="120"/>
+      <c r="U19" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V19" s="215">
         <v>45013</v>
       </c>
-      <c r="U19" s="215">
+      <c r="W19" s="215">
         <v>45015</v>
       </c>
-      <c r="V19" s="121"/>
-      <c r="W19" s="124"/>
-      <c r="X19" s="62"/>
-      <c r="Y19" s="122"/>
-      <c r="Z19" s="70"/>
-      <c r="AA19" s="27"/>
-      <c r="AB19" s="27"/>
+      <c r="X19" s="121"/>
+      <c r="Y19" s="124"/>
+      <c r="Z19" s="62"/>
+      <c r="AA19" s="122"/>
+      <c r="AB19" s="70"/>
       <c r="AC19" s="27"/>
       <c r="AD19" s="27"/>
       <c r="AE19" s="27"/>
@@ -22259,8 +22312,8 @@
       <c r="AJ19" s="27"/>
       <c r="AK19" s="27"/>
       <c r="AL19" s="27"/>
-      <c r="AM19" s="37"/>
-      <c r="AN19" s="37"/>
+      <c r="AM19" s="27"/>
+      <c r="AN19" s="27"/>
       <c r="AO19" s="37"/>
       <c r="AP19" s="37"/>
       <c r="AQ19" s="37"/>
@@ -22271,8 +22324,10 @@
       <c r="AV19" s="37"/>
       <c r="AW19" s="37"/>
       <c r="AX19" s="37"/>
+      <c r="AY19" s="37"/>
+      <c r="AZ19" s="37"/>
     </row>
-    <row r="20" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="71" t="s">
         <v>66</v>
       </c>
@@ -22319,26 +22374,26 @@
       <c r="P20" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="81"/>
-      <c r="S20" s="81" t="s">
+      <c r="Q20" s="150"/>
+      <c r="R20" s="150"/>
+      <c r="S20" s="81"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="81" t="s">
         <v>221</v>
       </c>
-      <c r="T20" s="214">
+      <c r="V20" s="214">
         <v>44862</v>
       </c>
-      <c r="U20" s="214">
+      <c r="W20" s="214">
         <v>44862</v>
       </c>
-      <c r="V20" s="81" t="s">
+      <c r="X20" s="81" t="s">
         <v>276</v>
       </c>
-      <c r="W20" s="81"/>
-      <c r="X20" s="81"/>
       <c r="Y20" s="81"/>
-      <c r="Z20" s="78"/>
-      <c r="AA20" s="27"/>
-      <c r="AB20" s="27"/>
+      <c r="Z20" s="81"/>
+      <c r="AA20" s="81"/>
+      <c r="AB20" s="78"/>
       <c r="AC20" s="27"/>
       <c r="AD20" s="27"/>
       <c r="AE20" s="27"/>
@@ -22349,8 +22404,8 @@
       <c r="AJ20" s="27"/>
       <c r="AK20" s="27"/>
       <c r="AL20" s="27"/>
-      <c r="AM20" s="37"/>
-      <c r="AN20" s="37"/>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="27"/>
       <c r="AO20" s="37"/>
       <c r="AP20" s="37"/>
       <c r="AQ20" s="37"/>
@@ -22361,8 +22416,10 @@
       <c r="AV20" s="37"/>
       <c r="AW20" s="37"/>
       <c r="AX20" s="37"/>
+      <c r="AY20" s="37"/>
+      <c r="AZ20" s="37"/>
     </row>
-    <row r="21" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="71" t="s">
         <v>72</v>
       </c>
@@ -22409,26 +22466,26 @@
       <c r="P21" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="81"/>
-      <c r="S21" s="120" t="s">
+      <c r="Q21" s="150"/>
+      <c r="R21" s="150"/>
+      <c r="S21" s="81"/>
+      <c r="T21" s="81"/>
+      <c r="U21" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T21" s="213">
+      <c r="V21" s="213">
         <v>44907</v>
       </c>
-      <c r="U21" s="214">
+      <c r="W21" s="214">
         <v>44914</v>
       </c>
-      <c r="V21" s="81"/>
-      <c r="W21" s="81"/>
       <c r="X21" s="81"/>
       <c r="Y21" s="81"/>
-      <c r="Z21" s="70" t="s">
+      <c r="Z21" s="81"/>
+      <c r="AA21" s="81"/>
+      <c r="AB21" s="70" t="s">
         <v>278</v>
       </c>
-      <c r="AA21" s="27"/>
-      <c r="AB21" s="27"/>
       <c r="AC21" s="27"/>
       <c r="AD21" s="27"/>
       <c r="AE21" s="27"/>
@@ -22439,8 +22496,8 @@
       <c r="AJ21" s="27"/>
       <c r="AK21" s="27"/>
       <c r="AL21" s="27"/>
-      <c r="AM21" s="37"/>
-      <c r="AN21" s="37"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="27"/>
       <c r="AO21" s="37"/>
       <c r="AP21" s="37"/>
       <c r="AQ21" s="37"/>
@@ -22451,8 +22508,10 @@
       <c r="AV21" s="37"/>
       <c r="AW21" s="37"/>
       <c r="AX21" s="37"/>
+      <c r="AY21" s="37"/>
+      <c r="AZ21" s="37"/>
     </row>
-    <row r="22" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="71" t="s">
         <v>72</v>
       </c>
@@ -22499,26 +22558,26 @@
       <c r="P22" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="81"/>
-      <c r="S22" s="120" t="s">
+      <c r="Q22" s="150"/>
+      <c r="R22" s="150"/>
+      <c r="S22" s="81"/>
+      <c r="T22" s="81"/>
+      <c r="U22" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T22" s="213">
+      <c r="V22" s="213">
         <v>44907</v>
       </c>
-      <c r="U22" s="214">
+      <c r="W22" s="214">
         <v>44914</v>
       </c>
-      <c r="V22" s="81"/>
-      <c r="W22" s="81"/>
       <c r="X22" s="81"/>
       <c r="Y22" s="81"/>
-      <c r="Z22" s="70" t="s">
+      <c r="Z22" s="81"/>
+      <c r="AA22" s="81"/>
+      <c r="AB22" s="70" t="s">
         <v>278</v>
       </c>
-      <c r="AA22" s="27"/>
-      <c r="AB22" s="27"/>
       <c r="AC22" s="27"/>
       <c r="AD22" s="27"/>
       <c r="AE22" s="27"/>
@@ -22529,8 +22588,8 @@
       <c r="AJ22" s="27"/>
       <c r="AK22" s="27"/>
       <c r="AL22" s="27"/>
-      <c r="AM22" s="37"/>
-      <c r="AN22" s="37"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="27"/>
       <c r="AO22" s="37"/>
       <c r="AP22" s="37"/>
       <c r="AQ22" s="37"/>
@@ -22541,8 +22600,10 @@
       <c r="AV22" s="37"/>
       <c r="AW22" s="37"/>
       <c r="AX22" s="37"/>
+      <c r="AY22" s="37"/>
+      <c r="AZ22" s="37"/>
     </row>
-    <row r="23" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="71" t="s">
         <v>66</v>
       </c>
@@ -22578,20 +22639,20 @@
       <c r="P23" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="Q23" s="81"/>
-      <c r="R23" s="81"/>
-      <c r="S23" s="120" t="s">
+      <c r="Q23" s="150"/>
+      <c r="R23" s="150"/>
+      <c r="S23" s="81"/>
+      <c r="T23" s="81"/>
+      <c r="U23" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T23" s="214"/>
-      <c r="U23" s="214"/>
-      <c r="V23" s="81"/>
-      <c r="W23" s="81"/>
+      <c r="V23" s="214"/>
+      <c r="W23" s="214"/>
       <c r="X23" s="81"/>
       <c r="Y23" s="81"/>
-      <c r="Z23" s="78"/>
-      <c r="AA23" s="27"/>
-      <c r="AB23" s="27"/>
+      <c r="Z23" s="81"/>
+      <c r="AA23" s="81"/>
+      <c r="AB23" s="78"/>
       <c r="AC23" s="27"/>
       <c r="AD23" s="27"/>
       <c r="AE23" s="27"/>
@@ -22602,8 +22663,8 @@
       <c r="AJ23" s="27"/>
       <c r="AK23" s="27"/>
       <c r="AL23" s="27"/>
-      <c r="AM23" s="37"/>
-      <c r="AN23" s="37"/>
+      <c r="AM23" s="27"/>
+      <c r="AN23" s="27"/>
       <c r="AO23" s="37"/>
       <c r="AP23" s="37"/>
       <c r="AQ23" s="37"/>
@@ -22614,8 +22675,10 @@
       <c r="AV23" s="37"/>
       <c r="AW23" s="37"/>
       <c r="AX23" s="37"/>
+      <c r="AY23" s="37"/>
+      <c r="AZ23" s="37"/>
     </row>
-    <row r="24" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="225" t="s">
         <v>66</v>
       </c>
@@ -22650,18 +22713,18 @@
       <c r="P24" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="Q24" s="81"/>
-      <c r="R24" s="81"/>
+      <c r="Q24" s="150"/>
+      <c r="R24" s="150"/>
       <c r="S24" s="81"/>
-      <c r="T24" s="214"/>
-      <c r="U24" s="214"/>
-      <c r="V24" s="81"/>
-      <c r="W24" s="81"/>
+      <c r="T24" s="81"/>
+      <c r="U24" s="81"/>
+      <c r="V24" s="214"/>
+      <c r="W24" s="214"/>
       <c r="X24" s="81"/>
       <c r="Y24" s="81"/>
-      <c r="Z24" s="78"/>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="27"/>
+      <c r="Z24" s="81"/>
+      <c r="AA24" s="81"/>
+      <c r="AB24" s="78"/>
       <c r="AC24" s="27"/>
       <c r="AD24" s="27"/>
       <c r="AE24" s="27"/>
@@ -22672,8 +22735,8 @@
       <c r="AJ24" s="27"/>
       <c r="AK24" s="27"/>
       <c r="AL24" s="27"/>
-      <c r="AM24" s="37"/>
-      <c r="AN24" s="37"/>
+      <c r="AM24" s="27"/>
+      <c r="AN24" s="27"/>
       <c r="AO24" s="37"/>
       <c r="AP24" s="37"/>
       <c r="AQ24" s="37"/>
@@ -22684,8 +22747,10 @@
       <c r="AV24" s="37"/>
       <c r="AW24" s="37"/>
       <c r="AX24" s="37"/>
+      <c r="AY24" s="37"/>
+      <c r="AZ24" s="37"/>
     </row>
-    <row r="25" spans="1:50" s="71" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" s="71" customFormat="1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="225" t="s">
         <v>66</v>
       </c>
@@ -22738,18 +22803,18 @@
       <c r="P25" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="Q25" s="81"/>
-      <c r="R25" s="81"/>
+      <c r="Q25" s="150"/>
+      <c r="R25" s="150"/>
       <c r="S25" s="81"/>
-      <c r="T25" s="214"/>
-      <c r="U25" s="214"/>
-      <c r="V25" s="81"/>
-      <c r="W25" s="81"/>
+      <c r="T25" s="81"/>
+      <c r="U25" s="81"/>
+      <c r="V25" s="214"/>
+      <c r="W25" s="214"/>
       <c r="X25" s="81"/>
       <c r="Y25" s="81"/>
-      <c r="Z25" s="78"/>
-      <c r="AA25" s="27"/>
-      <c r="AB25" s="27"/>
+      <c r="Z25" s="81"/>
+      <c r="AA25" s="81"/>
+      <c r="AB25" s="78"/>
       <c r="AC25" s="27"/>
       <c r="AD25" s="27"/>
       <c r="AE25" s="27"/>
@@ -22760,8 +22825,8 @@
       <c r="AJ25" s="27"/>
       <c r="AK25" s="27"/>
       <c r="AL25" s="27"/>
-      <c r="AM25" s="37"/>
-      <c r="AN25" s="37"/>
+      <c r="AM25" s="27"/>
+      <c r="AN25" s="27"/>
       <c r="AO25" s="37"/>
       <c r="AP25" s="37"/>
       <c r="AQ25" s="37"/>
@@ -22772,8 +22837,10 @@
       <c r="AV25" s="37"/>
       <c r="AW25" s="37"/>
       <c r="AX25" s="37"/>
+      <c r="AY25" s="37"/>
+      <c r="AZ25" s="37"/>
     </row>
-    <row r="26" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="71" t="s">
         <v>72</v>
       </c>
@@ -22820,22 +22887,22 @@
       <c r="P26" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q26" s="69"/>
-      <c r="R26" s="69"/>
-      <c r="S26" s="120" t="s">
+      <c r="Q26" s="150"/>
+      <c r="R26" s="150"/>
+      <c r="S26" s="69"/>
+      <c r="T26" s="69"/>
+      <c r="U26" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T26" s="212">
+      <c r="V26" s="212">
         <v>44901</v>
       </c>
-      <c r="U26" s="213"/>
-      <c r="V26" s="69"/>
-      <c r="W26" s="69"/>
+      <c r="W26" s="213"/>
       <c r="X26" s="69"/>
       <c r="Y26" s="69"/>
-      <c r="Z26" s="70"/>
-      <c r="AA26" s="27"/>
-      <c r="AB26" s="27"/>
+      <c r="Z26" s="69"/>
+      <c r="AA26" s="69"/>
+      <c r="AB26" s="70"/>
       <c r="AC26" s="27"/>
       <c r="AD26" s="27"/>
       <c r="AE26" s="27"/>
@@ -22846,8 +22913,8 @@
       <c r="AJ26" s="27"/>
       <c r="AK26" s="27"/>
       <c r="AL26" s="27"/>
-      <c r="AM26" s="37"/>
-      <c r="AN26" s="37"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="27"/>
       <c r="AO26" s="37"/>
       <c r="AP26" s="37"/>
       <c r="AQ26" s="37"/>
@@ -22858,8 +22925,10 @@
       <c r="AV26" s="37"/>
       <c r="AW26" s="37"/>
       <c r="AX26" s="37"/>
+      <c r="AY26" s="37"/>
+      <c r="AZ26" s="37"/>
     </row>
-    <row r="27" spans="1:50" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" s="71" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="71" t="s">
         <v>72</v>
       </c>
@@ -22906,26 +22975,26 @@
       <c r="P27" s="150" t="s">
         <v>223</v>
       </c>
-      <c r="Q27" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R27" s="81"/>
+      <c r="Q27" s="150"/>
+      <c r="R27" s="150"/>
       <c r="S27" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T27" s="212">
+      <c r="T27" s="81"/>
+      <c r="U27" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V27" s="212">
         <v>44901</v>
       </c>
-      <c r="U27" s="214">
+      <c r="W27" s="214">
         <v>44564</v>
       </c>
-      <c r="V27" s="81"/>
-      <c r="W27" s="81"/>
       <c r="X27" s="81"/>
       <c r="Y27" s="81"/>
-      <c r="Z27" s="78"/>
-      <c r="AA27" s="27"/>
-      <c r="AB27" s="27"/>
+      <c r="Z27" s="81"/>
+      <c r="AA27" s="81"/>
+      <c r="AB27" s="78"/>
       <c r="AC27" s="27"/>
       <c r="AD27" s="27"/>
       <c r="AE27" s="27"/>
@@ -22936,8 +23005,8 @@
       <c r="AJ27" s="27"/>
       <c r="AK27" s="27"/>
       <c r="AL27" s="27"/>
-      <c r="AM27" s="37"/>
-      <c r="AN27" s="37"/>
+      <c r="AM27" s="27"/>
+      <c r="AN27" s="27"/>
       <c r="AO27" s="37"/>
       <c r="AP27" s="37"/>
       <c r="AQ27" s="37"/>
@@ -22948,8 +23017,10 @@
       <c r="AV27" s="37"/>
       <c r="AW27" s="37"/>
       <c r="AX27" s="37"/>
+      <c r="AY27" s="37"/>
+      <c r="AZ27" s="37"/>
     </row>
-    <row r="28" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="71" t="s">
         <v>111</v>
       </c>
@@ -22997,26 +23068,26 @@
       <c r="P28" s="150" t="s">
         <v>220</v>
       </c>
-      <c r="Q28" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R28" s="120"/>
+      <c r="Q28" s="150"/>
+      <c r="R28" s="150"/>
       <c r="S28" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T28" s="215">
+      <c r="T28" s="120"/>
+      <c r="U28" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V28" s="215">
         <v>44895</v>
       </c>
-      <c r="U28" s="215">
+      <c r="W28" s="215">
         <v>44902</v>
       </c>
-      <c r="V28" s="121"/>
-      <c r="W28" s="121"/>
-      <c r="X28" s="64"/>
-      <c r="Y28" s="122"/>
-      <c r="Z28" s="70"/>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="27"/>
+      <c r="X28" s="121"/>
+      <c r="Y28" s="121"/>
+      <c r="Z28" s="64"/>
+      <c r="AA28" s="122"/>
+      <c r="AB28" s="70"/>
       <c r="AC28" s="27"/>
       <c r="AD28" s="27"/>
       <c r="AE28" s="27"/>
@@ -23027,8 +23098,8 @@
       <c r="AJ28" s="27"/>
       <c r="AK28" s="27"/>
       <c r="AL28" s="27"/>
-      <c r="AM28" s="37"/>
-      <c r="AN28" s="37"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="27"/>
       <c r="AO28" s="37"/>
       <c r="AP28" s="37"/>
       <c r="AQ28" s="37"/>
@@ -23039,8 +23110,10 @@
       <c r="AV28" s="37"/>
       <c r="AW28" s="37"/>
       <c r="AX28" s="37"/>
+      <c r="AY28" s="37"/>
+      <c r="AZ28" s="37"/>
     </row>
-    <row r="29" spans="1:50" s="170" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" s="170" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="71" t="s">
         <v>111</v>
       </c>
@@ -23088,26 +23161,26 @@
       <c r="P29" s="150" t="s">
         <v>220</v>
       </c>
-      <c r="Q29" s="120" t="s">
-        <v>221</v>
-      </c>
-      <c r="R29" s="120"/>
+      <c r="Q29" s="150"/>
+      <c r="R29" s="150"/>
       <c r="S29" s="120" t="s">
         <v>221</v>
       </c>
-      <c r="T29" s="215">
+      <c r="T29" s="120"/>
+      <c r="U29" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="V29" s="215">
         <v>44895</v>
       </c>
-      <c r="U29" s="215">
+      <c r="W29" s="215">
         <v>44902</v>
       </c>
-      <c r="V29" s="121"/>
-      <c r="W29" s="121"/>
-      <c r="X29" s="58"/>
-      <c r="Y29" s="122"/>
-      <c r="Z29" s="70"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="27"/>
+      <c r="X29" s="121"/>
+      <c r="Y29" s="121"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="122"/>
+      <c r="AB29" s="70"/>
       <c r="AC29" s="27"/>
       <c r="AD29" s="27"/>
       <c r="AE29" s="27"/>
@@ -23118,8 +23191,8 @@
       <c r="AJ29" s="27"/>
       <c r="AK29" s="27"/>
       <c r="AL29" s="27"/>
-      <c r="AM29" s="37"/>
-      <c r="AN29" s="37"/>
+      <c r="AM29" s="27"/>
+      <c r="AN29" s="27"/>
       <c r="AO29" s="37"/>
       <c r="AP29" s="37"/>
       <c r="AQ29" s="37"/>
@@ -23130,8 +23203,10 @@
       <c r="AV29" s="37"/>
       <c r="AW29" s="37"/>
       <c r="AX29" s="37"/>
+      <c r="AY29" s="37"/>
+      <c r="AZ29" s="37"/>
     </row>
-    <row r="30" spans="1:50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="285"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -23146,18 +23221,18 @@
       <c r="M30" s="7"/>
       <c r="N30" s="279"/>
       <c r="P30" s="278"/>
-      <c r="Q30" s="277"/>
-      <c r="R30" s="277"/>
+      <c r="Q30" s="278"/>
+      <c r="R30" s="278"/>
       <c r="S30" s="277"/>
-      <c r="T30" s="276"/>
-      <c r="U30" s="276"/>
-      <c r="V30" s="277"/>
-      <c r="W30" s="277"/>
+      <c r="T30" s="277"/>
+      <c r="U30" s="277"/>
+      <c r="V30" s="276"/>
+      <c r="W30" s="276"/>
       <c r="X30" s="277"/>
       <c r="Y30" s="277"/>
-      <c r="Z30" s="26"/>
-      <c r="AA30" s="275"/>
-      <c r="AB30" s="275"/>
+      <c r="Z30" s="277"/>
+      <c r="AA30" s="277"/>
+      <c r="AB30" s="26"/>
       <c r="AC30" s="275"/>
       <c r="AD30" s="275"/>
       <c r="AE30" s="275"/>
@@ -23168,8 +23243,8 @@
       <c r="AJ30" s="275"/>
       <c r="AK30" s="275"/>
       <c r="AL30" s="275"/>
-      <c r="AM30" s="274"/>
-      <c r="AN30" s="274"/>
+      <c r="AM30" s="275"/>
+      <c r="AN30" s="275"/>
       <c r="AO30" s="274"/>
       <c r="AP30" s="274"/>
       <c r="AQ30" s="274"/>
@@ -23180,8 +23255,10 @@
       <c r="AV30" s="274"/>
       <c r="AW30" s="274"/>
       <c r="AX30" s="274"/>
+      <c r="AY30" s="274"/>
+      <c r="AZ30" s="274"/>
     </row>
-    <row r="31" spans="1:50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="285"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -23196,18 +23273,18 @@
       <c r="M31" s="7"/>
       <c r="N31" s="279"/>
       <c r="P31" s="278"/>
-      <c r="Q31" s="277"/>
-      <c r="R31" s="277"/>
+      <c r="Q31" s="278"/>
+      <c r="R31" s="278"/>
       <c r="S31" s="277"/>
-      <c r="T31" s="276"/>
-      <c r="U31" s="276"/>
-      <c r="V31" s="277"/>
-      <c r="W31" s="277"/>
+      <c r="T31" s="277"/>
+      <c r="U31" s="277"/>
+      <c r="V31" s="276"/>
+      <c r="W31" s="276"/>
       <c r="X31" s="277"/>
       <c r="Y31" s="277"/>
-      <c r="Z31" s="26"/>
-      <c r="AA31" s="275"/>
-      <c r="AB31" s="275"/>
+      <c r="Z31" s="277"/>
+      <c r="AA31" s="277"/>
+      <c r="AB31" s="26"/>
       <c r="AC31" s="275"/>
       <c r="AD31" s="275"/>
       <c r="AE31" s="275"/>
@@ -23218,8 +23295,8 @@
       <c r="AJ31" s="275"/>
       <c r="AK31" s="275"/>
       <c r="AL31" s="275"/>
-      <c r="AM31" s="274"/>
-      <c r="AN31" s="274"/>
+      <c r="AM31" s="275"/>
+      <c r="AN31" s="275"/>
       <c r="AO31" s="274"/>
       <c r="AP31" s="274"/>
       <c r="AQ31" s="274"/>
@@ -23230,8 +23307,10 @@
       <c r="AV31" s="274"/>
       <c r="AW31" s="274"/>
       <c r="AX31" s="274"/>
+      <c r="AY31" s="274"/>
+      <c r="AZ31" s="274"/>
     </row>
-    <row r="32" spans="1:50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="285"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -23246,18 +23325,18 @@
       <c r="M32" s="7"/>
       <c r="N32" s="279"/>
       <c r="P32" s="278"/>
-      <c r="Q32" s="277"/>
-      <c r="R32" s="277"/>
+      <c r="Q32" s="278"/>
+      <c r="R32" s="278"/>
       <c r="S32" s="277"/>
-      <c r="T32" s="276"/>
-      <c r="U32" s="276"/>
-      <c r="V32" s="277"/>
-      <c r="W32" s="277"/>
+      <c r="T32" s="277"/>
+      <c r="U32" s="277"/>
+      <c r="V32" s="276"/>
+      <c r="W32" s="276"/>
       <c r="X32" s="277"/>
       <c r="Y32" s="277"/>
-      <c r="Z32" s="26"/>
-      <c r="AA32" s="275"/>
-      <c r="AB32" s="275"/>
+      <c r="Z32" s="277"/>
+      <c r="AA32" s="277"/>
+      <c r="AB32" s="26"/>
       <c r="AC32" s="275"/>
       <c r="AD32" s="275"/>
       <c r="AE32" s="275"/>
@@ -23268,8 +23347,8 @@
       <c r="AJ32" s="275"/>
       <c r="AK32" s="275"/>
       <c r="AL32" s="275"/>
-      <c r="AM32" s="274"/>
-      <c r="AN32" s="274"/>
+      <c r="AM32" s="275"/>
+      <c r="AN32" s="275"/>
       <c r="AO32" s="274"/>
       <c r="AP32" s="274"/>
       <c r="AQ32" s="274"/>
@@ -23280,8 +23359,10 @@
       <c r="AV32" s="274"/>
       <c r="AW32" s="274"/>
       <c r="AX32" s="274"/>
+      <c r="AY32" s="274"/>
+      <c r="AZ32" s="274"/>
     </row>
-    <row r="33" spans="1:52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:54" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="285"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -23296,18 +23377,18 @@
       <c r="M33" s="7"/>
       <c r="N33" s="279"/>
       <c r="P33" s="278"/>
-      <c r="Q33" s="277"/>
-      <c r="R33" s="277"/>
+      <c r="Q33" s="278"/>
+      <c r="R33" s="278"/>
       <c r="S33" s="277"/>
-      <c r="T33" s="276"/>
-      <c r="U33" s="276"/>
-      <c r="V33" s="277"/>
-      <c r="W33" s="277"/>
+      <c r="T33" s="277"/>
+      <c r="U33" s="277"/>
+      <c r="V33" s="276"/>
+      <c r="W33" s="276"/>
       <c r="X33" s="277"/>
       <c r="Y33" s="277"/>
-      <c r="Z33" s="26"/>
-      <c r="AA33" s="275"/>
-      <c r="AB33" s="275"/>
+      <c r="Z33" s="277"/>
+      <c r="AA33" s="277"/>
+      <c r="AB33" s="26"/>
       <c r="AC33" s="275"/>
       <c r="AD33" s="275"/>
       <c r="AE33" s="275"/>
@@ -23318,8 +23399,8 @@
       <c r="AJ33" s="275"/>
       <c r="AK33" s="275"/>
       <c r="AL33" s="275"/>
-      <c r="AM33" s="274"/>
-      <c r="AN33" s="274"/>
+      <c r="AM33" s="275"/>
+      <c r="AN33" s="275"/>
       <c r="AO33" s="274"/>
       <c r="AP33" s="274"/>
       <c r="AQ33" s="274"/>
@@ -23330,8 +23411,10 @@
       <c r="AV33" s="274"/>
       <c r="AW33" s="274"/>
       <c r="AX33" s="274"/>
+      <c r="AY33" s="274"/>
+      <c r="AZ33" s="274"/>
     </row>
-    <row r="34" spans="1:52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:54" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="285"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -23346,18 +23429,18 @@
       <c r="M34" s="7"/>
       <c r="N34" s="279"/>
       <c r="P34" s="278"/>
-      <c r="Q34" s="277"/>
-      <c r="R34" s="277"/>
+      <c r="Q34" s="278"/>
+      <c r="R34" s="278"/>
       <c r="S34" s="277"/>
-      <c r="T34" s="276"/>
-      <c r="U34" s="276"/>
-      <c r="V34" s="277"/>
-      <c r="W34" s="277"/>
+      <c r="T34" s="277"/>
+      <c r="U34" s="277"/>
+      <c r="V34" s="276"/>
+      <c r="W34" s="276"/>
       <c r="X34" s="277"/>
       <c r="Y34" s="277"/>
-      <c r="Z34" s="26"/>
-      <c r="AA34" s="275"/>
-      <c r="AB34" s="275"/>
+      <c r="Z34" s="277"/>
+      <c r="AA34" s="277"/>
+      <c r="AB34" s="26"/>
       <c r="AC34" s="275"/>
       <c r="AD34" s="275"/>
       <c r="AE34" s="275"/>
@@ -23368,8 +23451,8 @@
       <c r="AJ34" s="275"/>
       <c r="AK34" s="275"/>
       <c r="AL34" s="275"/>
-      <c r="AM34" s="274"/>
-      <c r="AN34" s="274"/>
+      <c r="AM34" s="275"/>
+      <c r="AN34" s="275"/>
       <c r="AO34" s="274"/>
       <c r="AP34" s="274"/>
       <c r="AQ34" s="274"/>
@@ -23380,8 +23463,10 @@
       <c r="AV34" s="274"/>
       <c r="AW34" s="274"/>
       <c r="AX34" s="274"/>
+      <c r="AY34" s="274"/>
+      <c r="AZ34" s="274"/>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="102"/>
       <c r="E35" s="102"/>
       <c r="F35" s="102"/>
@@ -23396,16 +23481,16 @@
       <c r="P35" s="102"/>
       <c r="Q35" s="102"/>
       <c r="R35" s="102"/>
-      <c r="S35" s="103"/>
+      <c r="S35" s="102"/>
       <c r="T35" s="102"/>
-      <c r="U35" s="102"/>
-      <c r="X35" s="102"/>
-      <c r="Y35" s="103"/>
+      <c r="U35" s="103"/>
+      <c r="V35" s="102"/>
+      <c r="W35" s="102"/>
       <c r="Z35" s="102"/>
-      <c r="AA35" s="104"/>
-      <c r="AB35" s="104"/>
-      <c r="AC35" s="102"/>
-      <c r="AD35" s="102"/>
+      <c r="AA35" s="103"/>
+      <c r="AB35" s="102"/>
+      <c r="AC35" s="104"/>
+      <c r="AD35" s="104"/>
       <c r="AE35" s="102"/>
       <c r="AF35" s="102"/>
       <c r="AG35" s="102"/>
@@ -23428,8 +23513,10 @@
       <c r="AX35" s="102"/>
       <c r="AY35" s="102"/>
       <c r="AZ35" s="102"/>
+      <c r="BA35" s="102"/>
+      <c r="BB35" s="102"/>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="102"/>
       <c r="E36" s="102"/>
       <c r="F36" s="102"/>
@@ -23444,16 +23531,16 @@
       <c r="P36" s="102"/>
       <c r="Q36" s="102"/>
       <c r="R36" s="102"/>
-      <c r="S36" s="103"/>
+      <c r="S36" s="102"/>
       <c r="T36" s="102"/>
-      <c r="U36" s="102"/>
-      <c r="X36" s="102"/>
-      <c r="Y36" s="103"/>
+      <c r="U36" s="103"/>
+      <c r="V36" s="102"/>
+      <c r="W36" s="102"/>
       <c r="Z36" s="102"/>
-      <c r="AA36" s="104"/>
-      <c r="AB36" s="104"/>
-      <c r="AC36" s="102"/>
-      <c r="AD36" s="102"/>
+      <c r="AA36" s="103"/>
+      <c r="AB36" s="102"/>
+      <c r="AC36" s="104"/>
+      <c r="AD36" s="104"/>
       <c r="AE36" s="102"/>
       <c r="AF36" s="102"/>
       <c r="AG36" s="102"/>
@@ -23476,8 +23563,10 @@
       <c r="AX36" s="102"/>
       <c r="AY36" s="102"/>
       <c r="AZ36" s="102"/>
+      <c r="BA36" s="102"/>
+      <c r="BB36" s="102"/>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="102"/>
       <c r="E37" s="102"/>
       <c r="F37" s="102"/>
@@ -23492,16 +23581,16 @@
       <c r="P37" s="102"/>
       <c r="Q37" s="102"/>
       <c r="R37" s="102"/>
-      <c r="S37" s="103"/>
+      <c r="S37" s="102"/>
       <c r="T37" s="102"/>
-      <c r="U37" s="102"/>
-      <c r="X37" s="102"/>
-      <c r="Y37" s="103"/>
+      <c r="U37" s="103"/>
+      <c r="V37" s="102"/>
+      <c r="W37" s="102"/>
       <c r="Z37" s="102"/>
-      <c r="AA37" s="104"/>
-      <c r="AB37" s="104"/>
-      <c r="AC37" s="102"/>
-      <c r="AD37" s="102"/>
+      <c r="AA37" s="103"/>
+      <c r="AB37" s="102"/>
+      <c r="AC37" s="104"/>
+      <c r="AD37" s="104"/>
       <c r="AE37" s="102"/>
       <c r="AF37" s="102"/>
       <c r="AG37" s="102"/>
@@ -23524,8 +23613,10 @@
       <c r="AX37" s="102"/>
       <c r="AY37" s="102"/>
       <c r="AZ37" s="102"/>
+      <c r="BA37" s="102"/>
+      <c r="BB37" s="102"/>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="102"/>
       <c r="E38" s="102"/>
       <c r="F38" s="102"/>
@@ -23540,16 +23631,16 @@
       <c r="P38" s="102"/>
       <c r="Q38" s="102"/>
       <c r="R38" s="102"/>
-      <c r="S38" s="103"/>
+      <c r="S38" s="102"/>
       <c r="T38" s="102"/>
-      <c r="U38" s="102"/>
-      <c r="X38" s="102"/>
-      <c r="Y38" s="103"/>
+      <c r="U38" s="103"/>
+      <c r="V38" s="102"/>
+      <c r="W38" s="102"/>
       <c r="Z38" s="102"/>
-      <c r="AA38" s="104"/>
-      <c r="AB38" s="104"/>
-      <c r="AC38" s="102"/>
-      <c r="AD38" s="102"/>
+      <c r="AA38" s="103"/>
+      <c r="AB38" s="102"/>
+      <c r="AC38" s="104"/>
+      <c r="AD38" s="104"/>
       <c r="AE38" s="102"/>
       <c r="AF38" s="102"/>
       <c r="AG38" s="102"/>
@@ -23572,8 +23663,10 @@
       <c r="AX38" s="102"/>
       <c r="AY38" s="102"/>
       <c r="AZ38" s="102"/>
+      <c r="BA38" s="102"/>
+      <c r="BB38" s="102"/>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="102"/>
       <c r="E39" s="102"/>
       <c r="F39" s="102"/>
@@ -23588,16 +23681,16 @@
       <c r="P39" s="102"/>
       <c r="Q39" s="102"/>
       <c r="R39" s="102"/>
-      <c r="S39" s="103"/>
+      <c r="S39" s="102"/>
       <c r="T39" s="102"/>
-      <c r="U39" s="102"/>
-      <c r="X39" s="102"/>
-      <c r="Y39" s="103"/>
+      <c r="U39" s="103"/>
+      <c r="V39" s="102"/>
+      <c r="W39" s="102"/>
       <c r="Z39" s="102"/>
-      <c r="AA39" s="104"/>
-      <c r="AB39" s="104"/>
-      <c r="AC39" s="102"/>
-      <c r="AD39" s="102"/>
+      <c r="AA39" s="103"/>
+      <c r="AB39" s="102"/>
+      <c r="AC39" s="104"/>
+      <c r="AD39" s="104"/>
       <c r="AE39" s="102"/>
       <c r="AF39" s="102"/>
       <c r="AG39" s="102"/>
@@ -23620,8 +23713,10 @@
       <c r="AX39" s="102"/>
       <c r="AY39" s="102"/>
       <c r="AZ39" s="102"/>
+      <c r="BA39" s="102"/>
+      <c r="BB39" s="102"/>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="102"/>
       <c r="E40" s="102"/>
       <c r="F40" s="102"/>
@@ -23636,16 +23731,16 @@
       <c r="P40" s="102"/>
       <c r="Q40" s="102"/>
       <c r="R40" s="102"/>
-      <c r="S40" s="103"/>
+      <c r="S40" s="102"/>
       <c r="T40" s="102"/>
-      <c r="U40" s="102"/>
-      <c r="X40" s="102"/>
-      <c r="Y40" s="103"/>
+      <c r="U40" s="103"/>
+      <c r="V40" s="102"/>
+      <c r="W40" s="102"/>
       <c r="Z40" s="102"/>
-      <c r="AA40" s="104"/>
-      <c r="AB40" s="104"/>
-      <c r="AC40" s="102"/>
-      <c r="AD40" s="102"/>
+      <c r="AA40" s="103"/>
+      <c r="AB40" s="102"/>
+      <c r="AC40" s="104"/>
+      <c r="AD40" s="104"/>
       <c r="AE40" s="102"/>
       <c r="AF40" s="102"/>
       <c r="AG40" s="102"/>
@@ -23668,8 +23763,10 @@
       <c r="AX40" s="102"/>
       <c r="AY40" s="102"/>
       <c r="AZ40" s="102"/>
+      <c r="BA40" s="102"/>
+      <c r="BB40" s="102"/>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="102"/>
       <c r="E41" s="102"/>
       <c r="F41" s="102"/>
@@ -23684,16 +23781,16 @@
       <c r="P41" s="102"/>
       <c r="Q41" s="102"/>
       <c r="R41" s="102"/>
-      <c r="S41" s="103"/>
+      <c r="S41" s="102"/>
       <c r="T41" s="102"/>
-      <c r="U41" s="102"/>
-      <c r="X41" s="102"/>
-      <c r="Y41" s="103"/>
+      <c r="U41" s="103"/>
+      <c r="V41" s="102"/>
+      <c r="W41" s="102"/>
       <c r="Z41" s="102"/>
-      <c r="AA41" s="104"/>
-      <c r="AB41" s="104"/>
-      <c r="AC41" s="102"/>
-      <c r="AD41" s="102"/>
+      <c r="AA41" s="103"/>
+      <c r="AB41" s="102"/>
+      <c r="AC41" s="104"/>
+      <c r="AD41" s="104"/>
       <c r="AE41" s="102"/>
       <c r="AF41" s="102"/>
       <c r="AG41" s="102"/>
@@ -23716,8 +23813,10 @@
       <c r="AX41" s="102"/>
       <c r="AY41" s="102"/>
       <c r="AZ41" s="102"/>
+      <c r="BA41" s="102"/>
+      <c r="BB41" s="102"/>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="102"/>
       <c r="E42" s="102"/>
       <c r="F42" s="102"/>
@@ -23732,16 +23831,16 @@
       <c r="P42" s="102"/>
       <c r="Q42" s="102"/>
       <c r="R42" s="102"/>
-      <c r="S42" s="103"/>
+      <c r="S42" s="102"/>
       <c r="T42" s="102"/>
-      <c r="U42" s="102"/>
-      <c r="X42" s="102"/>
-      <c r="Y42" s="103"/>
+      <c r="U42" s="103"/>
+      <c r="V42" s="102"/>
+      <c r="W42" s="102"/>
       <c r="Z42" s="102"/>
-      <c r="AA42" s="104"/>
-      <c r="AB42" s="104"/>
-      <c r="AC42" s="102"/>
-      <c r="AD42" s="102"/>
+      <c r="AA42" s="103"/>
+      <c r="AB42" s="102"/>
+      <c r="AC42" s="104"/>
+      <c r="AD42" s="104"/>
       <c r="AE42" s="102"/>
       <c r="AF42" s="102"/>
       <c r="AG42" s="102"/>
@@ -23764,8 +23863,10 @@
       <c r="AX42" s="102"/>
       <c r="AY42" s="102"/>
       <c r="AZ42" s="102"/>
+      <c r="BA42" s="102"/>
+      <c r="BB42" s="102"/>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="102"/>
       <c r="E43" s="102"/>
       <c r="F43" s="102"/>
@@ -23780,16 +23881,16 @@
       <c r="P43" s="102"/>
       <c r="Q43" s="102"/>
       <c r="R43" s="102"/>
-      <c r="S43" s="103"/>
+      <c r="S43" s="102"/>
       <c r="T43" s="102"/>
-      <c r="U43" s="102"/>
-      <c r="X43" s="102"/>
-      <c r="Y43" s="103"/>
+      <c r="U43" s="103"/>
+      <c r="V43" s="102"/>
+      <c r="W43" s="102"/>
       <c r="Z43" s="102"/>
-      <c r="AA43" s="104"/>
-      <c r="AB43" s="104"/>
-      <c r="AC43" s="102"/>
-      <c r="AD43" s="102"/>
+      <c r="AA43" s="103"/>
+      <c r="AB43" s="102"/>
+      <c r="AC43" s="104"/>
+      <c r="AD43" s="104"/>
       <c r="AE43" s="102"/>
       <c r="AF43" s="102"/>
       <c r="AG43" s="102"/>
@@ -23812,8 +23913,10 @@
       <c r="AX43" s="102"/>
       <c r="AY43" s="102"/>
       <c r="AZ43" s="102"/>
+      <c r="BA43" s="102"/>
+      <c r="BB43" s="102"/>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="102"/>
       <c r="E44" s="102"/>
       <c r="F44" s="102"/>
@@ -23828,16 +23931,16 @@
       <c r="P44" s="102"/>
       <c r="Q44" s="102"/>
       <c r="R44" s="102"/>
-      <c r="S44" s="103"/>
+      <c r="S44" s="102"/>
       <c r="T44" s="102"/>
-      <c r="U44" s="102"/>
-      <c r="X44" s="102"/>
-      <c r="Y44" s="103"/>
+      <c r="U44" s="103"/>
+      <c r="V44" s="102"/>
+      <c r="W44" s="102"/>
       <c r="Z44" s="102"/>
-      <c r="AA44" s="104"/>
-      <c r="AB44" s="104"/>
-      <c r="AC44" s="102"/>
-      <c r="AD44" s="102"/>
+      <c r="AA44" s="103"/>
+      <c r="AB44" s="102"/>
+      <c r="AC44" s="104"/>
+      <c r="AD44" s="104"/>
       <c r="AE44" s="102"/>
       <c r="AF44" s="102"/>
       <c r="AG44" s="102"/>
@@ -23860,8 +23963,10 @@
       <c r="AX44" s="102"/>
       <c r="AY44" s="102"/>
       <c r="AZ44" s="102"/>
+      <c r="BA44" s="102"/>
+      <c r="BB44" s="102"/>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="102"/>
       <c r="E45" s="102"/>
       <c r="F45" s="102"/>
@@ -23876,16 +23981,16 @@
       <c r="P45" s="102"/>
       <c r="Q45" s="102"/>
       <c r="R45" s="102"/>
-      <c r="S45" s="103"/>
+      <c r="S45" s="102"/>
       <c r="T45" s="102"/>
-      <c r="U45" s="102"/>
-      <c r="X45" s="102"/>
-      <c r="Y45" s="103"/>
+      <c r="U45" s="103"/>
+      <c r="V45" s="102"/>
+      <c r="W45" s="102"/>
       <c r="Z45" s="102"/>
-      <c r="AA45" s="104"/>
-      <c r="AB45" s="104"/>
-      <c r="AC45" s="102"/>
-      <c r="AD45" s="102"/>
+      <c r="AA45" s="103"/>
+      <c r="AB45" s="102"/>
+      <c r="AC45" s="104"/>
+      <c r="AD45" s="104"/>
       <c r="AE45" s="102"/>
       <c r="AF45" s="102"/>
       <c r="AG45" s="102"/>
@@ -23908,8 +24013,10 @@
       <c r="AX45" s="102"/>
       <c r="AY45" s="102"/>
       <c r="AZ45" s="102"/>
+      <c r="BA45" s="102"/>
+      <c r="BB45" s="102"/>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="102"/>
       <c r="E46" s="102"/>
       <c r="F46" s="102"/>
@@ -23924,16 +24031,16 @@
       <c r="P46" s="102"/>
       <c r="Q46" s="102"/>
       <c r="R46" s="102"/>
-      <c r="S46" s="103"/>
+      <c r="S46" s="102"/>
       <c r="T46" s="102"/>
-      <c r="U46" s="102"/>
-      <c r="X46" s="102"/>
-      <c r="Y46" s="103"/>
+      <c r="U46" s="103"/>
+      <c r="V46" s="102"/>
+      <c r="W46" s="102"/>
       <c r="Z46" s="102"/>
-      <c r="AA46" s="104"/>
-      <c r="AB46" s="104"/>
-      <c r="AC46" s="102"/>
-      <c r="AD46" s="102"/>
+      <c r="AA46" s="103"/>
+      <c r="AB46" s="102"/>
+      <c r="AC46" s="104"/>
+      <c r="AD46" s="104"/>
       <c r="AE46" s="102"/>
       <c r="AF46" s="102"/>
       <c r="AG46" s="102"/>
@@ -23956,8 +24063,10 @@
       <c r="AX46" s="102"/>
       <c r="AY46" s="102"/>
       <c r="AZ46" s="102"/>
+      <c r="BA46" s="102"/>
+      <c r="BB46" s="102"/>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="102"/>
       <c r="E47" s="102"/>
       <c r="F47" s="102"/>
@@ -23972,16 +24081,16 @@
       <c r="P47" s="102"/>
       <c r="Q47" s="102"/>
       <c r="R47" s="102"/>
-      <c r="S47" s="103"/>
+      <c r="S47" s="102"/>
       <c r="T47" s="102"/>
-      <c r="U47" s="102"/>
-      <c r="X47" s="102"/>
-      <c r="Y47" s="103"/>
+      <c r="U47" s="103"/>
+      <c r="V47" s="102"/>
+      <c r="W47" s="102"/>
       <c r="Z47" s="102"/>
-      <c r="AA47" s="104"/>
-      <c r="AB47" s="104"/>
-      <c r="AC47" s="102"/>
-      <c r="AD47" s="102"/>
+      <c r="AA47" s="103"/>
+      <c r="AB47" s="102"/>
+      <c r="AC47" s="104"/>
+      <c r="AD47" s="104"/>
       <c r="AE47" s="102"/>
       <c r="AF47" s="102"/>
       <c r="AG47" s="102"/>
@@ -24004,8 +24113,10 @@
       <c r="AX47" s="102"/>
       <c r="AY47" s="102"/>
       <c r="AZ47" s="102"/>
+      <c r="BA47" s="102"/>
+      <c r="BB47" s="102"/>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="102"/>
       <c r="E48" s="102"/>
       <c r="F48" s="102"/>
@@ -24020,16 +24131,16 @@
       <c r="P48" s="102"/>
       <c r="Q48" s="102"/>
       <c r="R48" s="102"/>
-      <c r="S48" s="103"/>
+      <c r="S48" s="102"/>
       <c r="T48" s="102"/>
-      <c r="U48" s="102"/>
-      <c r="X48" s="102"/>
-      <c r="Y48" s="103"/>
+      <c r="U48" s="103"/>
+      <c r="V48" s="102"/>
+      <c r="W48" s="102"/>
       <c r="Z48" s="102"/>
-      <c r="AA48" s="104"/>
-      <c r="AB48" s="104"/>
-      <c r="AC48" s="102"/>
-      <c r="AD48" s="102"/>
+      <c r="AA48" s="103"/>
+      <c r="AB48" s="102"/>
+      <c r="AC48" s="104"/>
+      <c r="AD48" s="104"/>
       <c r="AE48" s="102"/>
       <c r="AF48" s="102"/>
       <c r="AG48" s="102"/>
@@ -24052,8 +24163,10 @@
       <c r="AX48" s="102"/>
       <c r="AY48" s="102"/>
       <c r="AZ48" s="102"/>
+      <c r="BA48" s="102"/>
+      <c r="BB48" s="102"/>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="102"/>
       <c r="E49" s="102"/>
       <c r="F49" s="102"/>
@@ -24068,16 +24181,16 @@
       <c r="P49" s="102"/>
       <c r="Q49" s="102"/>
       <c r="R49" s="102"/>
-      <c r="S49" s="103"/>
+      <c r="S49" s="102"/>
       <c r="T49" s="102"/>
-      <c r="U49" s="102"/>
-      <c r="X49" s="102"/>
-      <c r="Y49" s="103"/>
+      <c r="U49" s="103"/>
+      <c r="V49" s="102"/>
+      <c r="W49" s="102"/>
       <c r="Z49" s="102"/>
-      <c r="AA49" s="104"/>
-      <c r="AB49" s="104"/>
-      <c r="AC49" s="102"/>
-      <c r="AD49" s="102"/>
+      <c r="AA49" s="103"/>
+      <c r="AB49" s="102"/>
+      <c r="AC49" s="104"/>
+      <c r="AD49" s="104"/>
       <c r="AE49" s="102"/>
       <c r="AF49" s="102"/>
       <c r="AG49" s="102"/>
@@ -24100,8 +24213,10 @@
       <c r="AX49" s="102"/>
       <c r="AY49" s="102"/>
       <c r="AZ49" s="102"/>
+      <c r="BA49" s="102"/>
+      <c r="BB49" s="102"/>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="102"/>
       <c r="E50" s="102"/>
       <c r="F50" s="102"/>
@@ -24116,16 +24231,16 @@
       <c r="P50" s="102"/>
       <c r="Q50" s="102"/>
       <c r="R50" s="102"/>
-      <c r="S50" s="103"/>
+      <c r="S50" s="102"/>
       <c r="T50" s="102"/>
-      <c r="U50" s="102"/>
-      <c r="X50" s="102"/>
-      <c r="Y50" s="103"/>
+      <c r="U50" s="103"/>
+      <c r="V50" s="102"/>
+      <c r="W50" s="102"/>
       <c r="Z50" s="102"/>
-      <c r="AA50" s="104"/>
-      <c r="AB50" s="104"/>
-      <c r="AC50" s="102"/>
-      <c r="AD50" s="102"/>
+      <c r="AA50" s="103"/>
+      <c r="AB50" s="102"/>
+      <c r="AC50" s="104"/>
+      <c r="AD50" s="104"/>
       <c r="AE50" s="102"/>
       <c r="AF50" s="102"/>
       <c r="AG50" s="102"/>
@@ -24148,8 +24263,10 @@
       <c r="AX50" s="102"/>
       <c r="AY50" s="102"/>
       <c r="AZ50" s="102"/>
+      <c r="BA50" s="102"/>
+      <c r="BB50" s="102"/>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="102"/>
       <c r="E51" s="102"/>
       <c r="F51" s="102"/>
@@ -24164,16 +24281,16 @@
       <c r="P51" s="102"/>
       <c r="Q51" s="102"/>
       <c r="R51" s="102"/>
-      <c r="S51" s="103"/>
+      <c r="S51" s="102"/>
       <c r="T51" s="102"/>
-      <c r="U51" s="102"/>
-      <c r="X51" s="102"/>
-      <c r="Y51" s="103"/>
+      <c r="U51" s="103"/>
+      <c r="V51" s="102"/>
+      <c r="W51" s="102"/>
       <c r="Z51" s="102"/>
-      <c r="AA51" s="104"/>
-      <c r="AB51" s="104"/>
-      <c r="AC51" s="102"/>
-      <c r="AD51" s="102"/>
+      <c r="AA51" s="103"/>
+      <c r="AB51" s="102"/>
+      <c r="AC51" s="104"/>
+      <c r="AD51" s="104"/>
       <c r="AE51" s="102"/>
       <c r="AF51" s="102"/>
       <c r="AG51" s="102"/>
@@ -24196,8 +24313,10 @@
       <c r="AX51" s="102"/>
       <c r="AY51" s="102"/>
       <c r="AZ51" s="102"/>
+      <c r="BA51" s="102"/>
+      <c r="BB51" s="102"/>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="102"/>
       <c r="E52" s="102"/>
       <c r="F52" s="102"/>
@@ -24212,16 +24331,16 @@
       <c r="P52" s="102"/>
       <c r="Q52" s="102"/>
       <c r="R52" s="102"/>
-      <c r="S52" s="103"/>
+      <c r="S52" s="102"/>
       <c r="T52" s="102"/>
-      <c r="U52" s="102"/>
-      <c r="X52" s="102"/>
-      <c r="Y52" s="103"/>
+      <c r="U52" s="103"/>
+      <c r="V52" s="102"/>
+      <c r="W52" s="102"/>
       <c r="Z52" s="102"/>
-      <c r="AA52" s="104"/>
-      <c r="AB52" s="104"/>
-      <c r="AC52" s="102"/>
-      <c r="AD52" s="102"/>
+      <c r="AA52" s="103"/>
+      <c r="AB52" s="102"/>
+      <c r="AC52" s="104"/>
+      <c r="AD52" s="104"/>
       <c r="AE52" s="102"/>
       <c r="AF52" s="102"/>
       <c r="AG52" s="102"/>
@@ -24244,8 +24363,10 @@
       <c r="AX52" s="102"/>
       <c r="AY52" s="102"/>
       <c r="AZ52" s="102"/>
+      <c r="BA52" s="102"/>
+      <c r="BB52" s="102"/>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="102"/>
       <c r="E53" s="102"/>
       <c r="F53" s="102"/>
@@ -24260,16 +24381,16 @@
       <c r="P53" s="102"/>
       <c r="Q53" s="102"/>
       <c r="R53" s="102"/>
-      <c r="S53" s="103"/>
+      <c r="S53" s="102"/>
       <c r="T53" s="102"/>
-      <c r="U53" s="102"/>
-      <c r="X53" s="102"/>
-      <c r="Y53" s="103"/>
+      <c r="U53" s="103"/>
+      <c r="V53" s="102"/>
+      <c r="W53" s="102"/>
       <c r="Z53" s="102"/>
-      <c r="AA53" s="104"/>
-      <c r="AB53" s="104"/>
-      <c r="AC53" s="102"/>
-      <c r="AD53" s="102"/>
+      <c r="AA53" s="103"/>
+      <c r="AB53" s="102"/>
+      <c r="AC53" s="104"/>
+      <c r="AD53" s="104"/>
       <c r="AE53" s="102"/>
       <c r="AF53" s="102"/>
       <c r="AG53" s="102"/>
@@ -24292,8 +24413,10 @@
       <c r="AX53" s="102"/>
       <c r="AY53" s="102"/>
       <c r="AZ53" s="102"/>
+      <c r="BA53" s="102"/>
+      <c r="BB53" s="102"/>
     </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="102"/>
       <c r="E54" s="102"/>
       <c r="F54" s="102"/>
@@ -24308,16 +24431,16 @@
       <c r="P54" s="102"/>
       <c r="Q54" s="102"/>
       <c r="R54" s="102"/>
-      <c r="S54" s="103"/>
+      <c r="S54" s="102"/>
       <c r="T54" s="102"/>
-      <c r="U54" s="102"/>
-      <c r="X54" s="102"/>
-      <c r="Y54" s="103"/>
+      <c r="U54" s="103"/>
+      <c r="V54" s="102"/>
+      <c r="W54" s="102"/>
       <c r="Z54" s="102"/>
-      <c r="AA54" s="104"/>
-      <c r="AB54" s="104"/>
-      <c r="AC54" s="102"/>
-      <c r="AD54" s="102"/>
+      <c r="AA54" s="103"/>
+      <c r="AB54" s="102"/>
+      <c r="AC54" s="104"/>
+      <c r="AD54" s="104"/>
       <c r="AE54" s="102"/>
       <c r="AF54" s="102"/>
       <c r="AG54" s="102"/>
@@ -24340,8 +24463,10 @@
       <c r="AX54" s="102"/>
       <c r="AY54" s="102"/>
       <c r="AZ54" s="102"/>
+      <c r="BA54" s="102"/>
+      <c r="BB54" s="102"/>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="102"/>
       <c r="E55" s="102"/>
       <c r="F55" s="102"/>
@@ -24356,16 +24481,16 @@
       <c r="P55" s="102"/>
       <c r="Q55" s="102"/>
       <c r="R55" s="102"/>
-      <c r="S55" s="103"/>
+      <c r="S55" s="102"/>
       <c r="T55" s="102"/>
-      <c r="U55" s="102"/>
-      <c r="X55" s="102"/>
-      <c r="Y55" s="103"/>
+      <c r="U55" s="103"/>
+      <c r="V55" s="102"/>
+      <c r="W55" s="102"/>
       <c r="Z55" s="102"/>
-      <c r="AA55" s="104"/>
-      <c r="AB55" s="104"/>
-      <c r="AC55" s="102"/>
-      <c r="AD55" s="102"/>
+      <c r="AA55" s="103"/>
+      <c r="AB55" s="102"/>
+      <c r="AC55" s="104"/>
+      <c r="AD55" s="104"/>
       <c r="AE55" s="102"/>
       <c r="AF55" s="102"/>
       <c r="AG55" s="102"/>
@@ -24388,8 +24513,10 @@
       <c r="AX55" s="102"/>
       <c r="AY55" s="102"/>
       <c r="AZ55" s="102"/>
+      <c r="BA55" s="102"/>
+      <c r="BB55" s="102"/>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="102"/>
       <c r="E56" s="102"/>
       <c r="F56" s="102"/>
@@ -24404,16 +24531,16 @@
       <c r="P56" s="102"/>
       <c r="Q56" s="102"/>
       <c r="R56" s="102"/>
-      <c r="S56" s="103"/>
+      <c r="S56" s="102"/>
       <c r="T56" s="102"/>
-      <c r="U56" s="102"/>
-      <c r="X56" s="102"/>
-      <c r="Y56" s="103"/>
+      <c r="U56" s="103"/>
+      <c r="V56" s="102"/>
+      <c r="W56" s="102"/>
       <c r="Z56" s="102"/>
-      <c r="AA56" s="104"/>
-      <c r="AB56" s="104"/>
-      <c r="AC56" s="102"/>
-      <c r="AD56" s="102"/>
+      <c r="AA56" s="103"/>
+      <c r="AB56" s="102"/>
+      <c r="AC56" s="104"/>
+      <c r="AD56" s="104"/>
       <c r="AE56" s="102"/>
       <c r="AF56" s="102"/>
       <c r="AG56" s="102"/>
@@ -24436,8 +24563,10 @@
       <c r="AX56" s="102"/>
       <c r="AY56" s="102"/>
       <c r="AZ56" s="102"/>
+      <c r="BA56" s="102"/>
+      <c r="BB56" s="102"/>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="102"/>
       <c r="E57" s="102"/>
       <c r="F57" s="102"/>
@@ -24452,16 +24581,16 @@
       <c r="P57" s="102"/>
       <c r="Q57" s="102"/>
       <c r="R57" s="102"/>
-      <c r="S57" s="103"/>
+      <c r="S57" s="102"/>
       <c r="T57" s="102"/>
-      <c r="U57" s="102"/>
-      <c r="X57" s="102"/>
-      <c r="Y57" s="103"/>
+      <c r="U57" s="103"/>
+      <c r="V57" s="102"/>
+      <c r="W57" s="102"/>
       <c r="Z57" s="102"/>
-      <c r="AA57" s="104"/>
-      <c r="AB57" s="104"/>
-      <c r="AC57" s="102"/>
-      <c r="AD57" s="102"/>
+      <c r="AA57" s="103"/>
+      <c r="AB57" s="102"/>
+      <c r="AC57" s="104"/>
+      <c r="AD57" s="104"/>
       <c r="AE57" s="102"/>
       <c r="AF57" s="102"/>
       <c r="AG57" s="102"/>
@@ -24484,8 +24613,10 @@
       <c r="AX57" s="102"/>
       <c r="AY57" s="102"/>
       <c r="AZ57" s="102"/>
+      <c r="BA57" s="102"/>
+      <c r="BB57" s="102"/>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="102"/>
       <c r="E58" s="102"/>
       <c r="F58" s="102"/>
@@ -24500,16 +24631,16 @@
       <c r="P58" s="102"/>
       <c r="Q58" s="102"/>
       <c r="R58" s="102"/>
-      <c r="S58" s="103"/>
+      <c r="S58" s="102"/>
       <c r="T58" s="102"/>
-      <c r="U58" s="102"/>
-      <c r="X58" s="102"/>
-      <c r="Y58" s="103"/>
+      <c r="U58" s="103"/>
+      <c r="V58" s="102"/>
+      <c r="W58" s="102"/>
       <c r="Z58" s="102"/>
-      <c r="AA58" s="104"/>
-      <c r="AB58" s="104"/>
-      <c r="AC58" s="102"/>
-      <c r="AD58" s="102"/>
+      <c r="AA58" s="103"/>
+      <c r="AB58" s="102"/>
+      <c r="AC58" s="104"/>
+      <c r="AD58" s="104"/>
       <c r="AE58" s="102"/>
       <c r="AF58" s="102"/>
       <c r="AG58" s="102"/>
@@ -24532,8 +24663,10 @@
       <c r="AX58" s="102"/>
       <c r="AY58" s="102"/>
       <c r="AZ58" s="102"/>
+      <c r="BA58" s="102"/>
+      <c r="BB58" s="102"/>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="102"/>
       <c r="E59" s="102"/>
       <c r="F59" s="102"/>
@@ -24548,16 +24681,16 @@
       <c r="P59" s="102"/>
       <c r="Q59" s="102"/>
       <c r="R59" s="102"/>
-      <c r="S59" s="103"/>
+      <c r="S59" s="102"/>
       <c r="T59" s="102"/>
-      <c r="U59" s="102"/>
-      <c r="X59" s="102"/>
-      <c r="Y59" s="103"/>
+      <c r="U59" s="103"/>
+      <c r="V59" s="102"/>
+      <c r="W59" s="102"/>
       <c r="Z59" s="102"/>
-      <c r="AA59" s="104"/>
-      <c r="AB59" s="104"/>
-      <c r="AC59" s="102"/>
-      <c r="AD59" s="102"/>
+      <c r="AA59" s="103"/>
+      <c r="AB59" s="102"/>
+      <c r="AC59" s="104"/>
+      <c r="AD59" s="104"/>
       <c r="AE59" s="102"/>
       <c r="AF59" s="102"/>
       <c r="AG59" s="102"/>
@@ -24580,8 +24713,10 @@
       <c r="AX59" s="102"/>
       <c r="AY59" s="102"/>
       <c r="AZ59" s="102"/>
+      <c r="BA59" s="102"/>
+      <c r="BB59" s="102"/>
     </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="102"/>
       <c r="E60" s="102"/>
       <c r="F60" s="102"/>
@@ -24596,16 +24731,16 @@
       <c r="P60" s="102"/>
       <c r="Q60" s="102"/>
       <c r="R60" s="102"/>
-      <c r="S60" s="103"/>
+      <c r="S60" s="102"/>
       <c r="T60" s="102"/>
-      <c r="U60" s="102"/>
-      <c r="X60" s="102"/>
-      <c r="Y60" s="103"/>
+      <c r="U60" s="103"/>
+      <c r="V60" s="102"/>
+      <c r="W60" s="102"/>
       <c r="Z60" s="102"/>
-      <c r="AA60" s="104"/>
-      <c r="AB60" s="104"/>
-      <c r="AC60" s="102"/>
-      <c r="AD60" s="102"/>
+      <c r="AA60" s="103"/>
+      <c r="AB60" s="102"/>
+      <c r="AC60" s="104"/>
+      <c r="AD60" s="104"/>
       <c r="AE60" s="102"/>
       <c r="AF60" s="102"/>
       <c r="AG60" s="102"/>
@@ -24628,8 +24763,10 @@
       <c r="AX60" s="102"/>
       <c r="AY60" s="102"/>
       <c r="AZ60" s="102"/>
+      <c r="BA60" s="102"/>
+      <c r="BB60" s="102"/>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:54" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="102"/>
       <c r="E61" s="102"/>
       <c r="F61" s="102"/>
@@ -24644,16 +24781,16 @@
       <c r="P61" s="102"/>
       <c r="Q61" s="102"/>
       <c r="R61" s="102"/>
-      <c r="S61" s="103"/>
+      <c r="S61" s="102"/>
       <c r="T61" s="102"/>
-      <c r="U61" s="102"/>
-      <c r="X61" s="102"/>
-      <c r="Y61" s="103"/>
+      <c r="U61" s="103"/>
+      <c r="V61" s="102"/>
+      <c r="W61" s="102"/>
       <c r="Z61" s="102"/>
-      <c r="AA61" s="104"/>
-      <c r="AB61" s="104"/>
-      <c r="AC61" s="102"/>
-      <c r="AD61" s="102"/>
+      <c r="AA61" s="103"/>
+      <c r="AB61" s="102"/>
+      <c r="AC61" s="104"/>
+      <c r="AD61" s="104"/>
       <c r="AE61" s="102"/>
       <c r="AF61" s="102"/>
       <c r="AG61" s="102"/>
@@ -24676,10 +24813,12 @@
       <c r="AX61" s="102"/>
       <c r="AY61" s="102"/>
       <c r="AZ61" s="102"/>
+      <c r="BA61" s="102"/>
+      <c r="BB61" s="102"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AX29" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AX29">
+  <autoFilter ref="A1:AZ29" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AZ29">
     <sortCondition ref="B3:B29"/>
   </sortState>
   <phoneticPr fontId="34" type="noConversion"/>
@@ -24699,7 +24838,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>